<commit_message>
create seperate view for underwriter and sales executive.
</commit_message>
<xml_diff>
--- a/IntranetPortal/IntranetPortal/TempDataFile/underwriter.xlsx
+++ b/IntranetPortal/IntranetPortal/TempDataFile/underwriter.xlsx
@@ -56,7 +56,7 @@
     <x:t>Property Address:</x:t>
   </x:si>
   <x:si>
-    <x:t>3 E 128 ST, Manhattan,NY 10035</x:t>
+    <x:t>122-14 134 ST, SOUTH OZONE PARK,NY 11420</x:t>
   </x:si>
   <x:si>
     <x:t>1st Mortgage</x:t>
@@ -80,12 +80,15 @@
     <x:t>Building Dimension</x:t>
   </x:si>
   <x:si>
-    <x:t>20'x63'</x:t>
+    <x:t>24'x50'</x:t>
   </x:si>
   <x:si>
     <x:t>COS Recorded:</x:t>
   </x:si>
   <x:si>
+    <x:t>No</x:t>
+  </x:si>
+  <x:si>
     <x:t>Water Charges:</x:t>
   </x:si>
   <x:si>
@@ -107,7 +110,7 @@
     <x:t>Zoning</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">R7-2     </x:t>
+    <x:t xml:space="preserve">R3-2     </x:t>
   </x:si>
   <x:si>
     <x:t>Other Liens:</x:t>
@@ -125,9 +128,6 @@
     <x:t>FHA:</x:t>
   </x:si>
   <x:si>
-    <x:t>No</x:t>
-  </x:si>
-  <x:si>
     <x:t>DOB Civil Penalty</x:t>
   </x:si>
   <x:si>
@@ -174,6 +174,9 @@
   </x:si>
   <x:si>
     <x:t>Vacate Order:</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Yes</x:t>
   </x:si>
   <x:si>
     <x:t>BEST CASE SCENARIO</x:t>
@@ -652,9 +655,6 @@
   </x:si>
   <x:si>
     <x:t>Points</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Yes</x:t>
   </x:si>
   <x:si>
     <x:t>Flip ROI</x:t>
@@ -4644,7 +4644,9 @@
       <x:c r="E3" s="243" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="F3" s="290" t="s"/>
+      <x:c r="F3" s="290" t="n">
+        <x:v>0</x:v>
+      </x:c>
       <x:c r="G3" s="358" t="s"/>
       <x:c r="H3" s="244" t="s">
         <x:v>7</x:v>
@@ -4673,12 +4675,16 @@
       <x:c r="E4" s="243" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F4" s="290" t="s"/>
+      <x:c r="F4" s="290" t="n">
+        <x:v>0</x:v>
+      </x:c>
       <x:c r="G4" s="358" t="s"/>
       <x:c r="H4" s="244" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="I4" s="281" t="s"/>
+      <x:c r="I4" s="281" t="n">
+        <x:v>0</x:v>
+      </x:c>
       <x:c r="J4" s="357" t="s"/>
       <x:c r="K4" s="357" t="s"/>
       <x:c r="L4" s="362" t="s"/>
@@ -4696,15 +4702,17 @@
       <x:c r="E5" s="244" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="F5" s="279" t="s"/>
+      <x:c r="F5" s="279" t="s">
+        <x:v>15</x:v>
+      </x:c>
       <x:c r="G5" s="358" t="s"/>
       <x:c r="H5" s="244" t="s">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="I5" s="281" t="s"/>
       <x:c r="J5" s="357" t="s"/>
       <x:c r="K5" s="370" t="s">
-        <x:v>16</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="L5" s="371" t="s"/>
       <x:c r="M5" s="357" t="s"/>
@@ -4713,24 +4721,26 @@
     <x:row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <x:c r="A6" s="357" t="s"/>
       <x:c r="B6" s="359" t="s">
-        <x:v>17</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="C6" s="274" t="n">
-        <x:v>5</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="D6" s="358" t="s"/>
       <x:c r="E6" s="244" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="F6" s="279" t="s"/>
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="F6" s="279" t="s">
+        <x:v>15</x:v>
+      </x:c>
       <x:c r="G6" s="358" t="s"/>
       <x:c r="H6" s="244" t="s">
-        <x:v>19</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="I6" s="281" t="s"/>
       <x:c r="J6" s="357" t="s"/>
       <x:c r="K6" s="373" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="L6" s="374" t="e">
         <x:f>SUM(Tables!K6:K22)</x:f>
@@ -4740,24 +4750,24 @@
     <x:row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <x:c r="A7" s="357" t="s"/>
       <x:c r="B7" s="359" t="s">
-        <x:v>21</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="C7" s="274" t="s">
-        <x:v>22</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="D7" s="358" t="s"/>
       <x:c r="E7" s="244" t="s">
-        <x:v>23</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="F7" s="279" t="s"/>
       <x:c r="G7" s="358" t="s"/>
       <x:c r="H7" s="244" t="s">
-        <x:v>24</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="I7" s="281" t="s"/>
       <x:c r="J7" s="357" t="s"/>
       <x:c r="K7" s="375" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="L7" s="376" t="e">
         <x:f>'Flip Sheets'!C26</x:f>
@@ -4767,15 +4777,15 @@
     <x:row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <x:c r="A8" s="357" t="s"/>
       <x:c r="B8" s="244" t="s">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="C8" s="277" t="s"/>
       <x:c r="D8" s="358" t="s"/>
       <x:c r="E8" s="244" t="s">
-        <x:v>27</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="F8" s="279" t="s">
-        <x:v>28</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="G8" s="358" t="s"/>
       <x:c r="H8" s="244" t="s">
@@ -4802,7 +4812,7 @@
         <x:v>32</x:v>
       </x:c>
       <x:c r="F9" s="279" t="s">
-        <x:v>28</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="G9" s="358" t="s"/>
       <x:c r="H9" s="244" t="s">
@@ -4828,7 +4838,9 @@
       <x:c r="E10" s="244" t="s">
         <x:v>36</x:v>
       </x:c>
-      <x:c r="F10" s="279" t="s"/>
+      <x:c r="F10" s="279" t="s">
+        <x:v>15</x:v>
+      </x:c>
       <x:c r="G10" s="358" t="s"/>
       <x:c r="H10" s="244" t="s">
         <x:v>37</x:v>
@@ -4881,10 +4893,12 @@
       <x:c r="H12" s="244" t="s">
         <x:v>44</x:v>
       </x:c>
-      <x:c r="I12" s="287" t="s"/>
+      <x:c r="I12" s="287" t="s">
+        <x:v>45</x:v>
+      </x:c>
       <x:c r="J12" s="357" t="s"/>
       <x:c r="K12" s="360" t="s">
-        <x:v>45</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="L12" s="361" t="s"/>
       <x:c r="M12" s="357" t="s"/>
@@ -4895,17 +4909,19 @@
       <x:c r="C13" s="358" t="s"/>
       <x:c r="D13" s="358" t="s"/>
       <x:c r="E13" s="244" t="s">
-        <x:v>46</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="F13" s="291" t="s"/>
       <x:c r="G13" s="357" t="s"/>
       <x:c r="H13" s="244" t="s">
-        <x:v>47</x:v>
-      </x:c>
-      <x:c r="I13" s="281" t="s"/>
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="I13" s="281" t="n">
+        <x:v>0</x:v>
+      </x:c>
       <x:c r="J13" s="357" t="s"/>
       <x:c r="K13" s="382" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="L13" s="383">
         <x:f>C21+SUM(Tables!K9:K22)</x:f>
@@ -4915,22 +4931,22 @@
     <x:row r="14" spans="1:15" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A14" s="357" t="s"/>
       <x:c r="B14" s="384" t="s">
-        <x:v>48</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="C14" s="385" t="s"/>
       <x:c r="D14" s="386" t="s"/>
       <x:c r="E14" s="244" t="s">
-        <x:v>49</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="F14" s="275" t="s"/>
       <x:c r="G14" s="358" t="s"/>
       <x:c r="H14" s="387" t="s">
-        <x:v>50</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="I14" s="388" t="s"/>
       <x:c r="J14" s="357" t="s"/>
       <x:c r="K14" s="389" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="L14" s="390" t="e">
         <x:f>(L13+SUM('Flip Sheets'!$C$21:$C$25))</x:f>
@@ -4940,12 +4956,12 @@
     <x:row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <x:c r="A15" s="357" t="s"/>
       <x:c r="B15" s="244" t="s">
-        <x:v>51</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="C15" s="281" t="s"/>
       <x:c r="D15" s="386" t="s"/>
       <x:c r="E15" s="243" t="s">
-        <x:v>52</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="F15" s="391" t="s"/>
       <x:c r="G15" s="358" t="s"/>
@@ -4963,12 +4979,12 @@
     <x:row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <x:c r="A16" s="357" t="s"/>
       <x:c r="B16" s="244" t="s">
-        <x:v>53</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="C16" s="281" t="s"/>
       <x:c r="D16" s="357" t="s"/>
       <x:c r="E16" s="244" t="s">
-        <x:v>54</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="F16" s="294" t="s"/>
       <x:c r="G16" s="358" t="s"/>
@@ -4986,12 +5002,12 @@
     <x:row r="17" spans="1:15" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A17" s="357" t="s"/>
       <x:c r="B17" s="243" t="s">
-        <x:v>55</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="C17" s="394" t="s"/>
       <x:c r="D17" s="386" t="s"/>
       <x:c r="E17" s="244" t="s">
-        <x:v>56</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="F17" s="278" t="s"/>
       <x:c r="G17" s="358" t="s"/>
@@ -5009,12 +5025,12 @@
     <x:row r="18" spans="1:15" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A18" s="357" t="s"/>
       <x:c r="B18" s="397" t="s">
-        <x:v>57</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="C18" s="283" t="s"/>
       <x:c r="D18" s="358" t="s"/>
       <x:c r="E18" s="244" t="s">
-        <x:v>58</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="F18" s="294" t="s"/>
       <x:c r="G18" s="357" t="s"/>
@@ -5031,7 +5047,7 @@
       <x:c r="C19" s="398" t="s"/>
       <x:c r="D19" s="358" t="s"/>
       <x:c r="E19" s="248" t="s">
-        <x:v>59</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="F19" s="295" t="s"/>
       <x:c r="G19" s="357" t="s"/>
@@ -5039,7 +5055,7 @@
       <x:c r="I19" s="392" t="s"/>
       <x:c r="J19" s="357" t="s"/>
       <x:c r="K19" s="399" t="s">
-        <x:v>60</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="L19" s="400" t="s"/>
       <x:c r="M19" s="357" t="s"/>
@@ -5047,7 +5063,7 @@
     <x:row r="20" spans="1:15" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A20" s="357" t="s"/>
       <x:c r="B20" s="365" t="s">
-        <x:v>61</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="C20" s="401" t="s"/>
       <x:c r="D20" s="358" t="s"/>
@@ -5058,7 +5074,7 @@
       <x:c r="I20" s="357" t="s"/>
       <x:c r="J20" s="357" t="s"/>
       <x:c r="K20" s="402" t="s">
-        <x:v>62</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="L20" s="403">
         <x:f>'Rental Model'!C9</x:f>
@@ -5068,12 +5084,12 @@
     <x:row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <x:c r="A21" s="357" t="s"/>
       <x:c r="B21" s="243" t="s">
-        <x:v>63</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="C21" s="394" t="s"/>
       <x:c r="D21" s="358" t="s"/>
       <x:c r="E21" s="404" t="s">
-        <x:v>64</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="F21" s="405" t="s"/>
       <x:c r="G21" s="405" t="s"/>
@@ -5081,7 +5097,7 @@
       <x:c r="I21" s="406" t="s"/>
       <x:c r="J21" s="357" t="s"/>
       <x:c r="K21" s="407" t="s">
-        <x:v>65</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="L21" s="403">
         <x:f>'Rental Model'!F11</x:f>
@@ -5091,7 +5107,7 @@
     <x:row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <x:c r="A22" s="357" t="s"/>
       <x:c r="B22" s="244" t="s">
-        <x:v>66</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="C22" s="281" t="s"/>
       <x:c r="D22" s="358" t="s"/>
@@ -5102,7 +5118,7 @@
       <x:c r="I22" s="410" t="s"/>
       <x:c r="J22" s="357" t="s"/>
       <x:c r="K22" s="407" t="s">
-        <x:v>67</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="L22" s="411" t="e">
         <x:f>'Rental Model'!H3</x:f>
@@ -5112,7 +5128,7 @@
     <x:row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <x:c r="A23" s="357" t="s"/>
       <x:c r="B23" s="244" t="s">
-        <x:v>68</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="C23" s="281" t="s"/>
       <x:c r="D23" s="358" t="s"/>
@@ -5123,7 +5139,7 @@
       <x:c r="I23" s="410" t="s"/>
       <x:c r="J23" s="357" t="s"/>
       <x:c r="K23" s="407" t="s">
-        <x:v>69</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="L23" s="412" t="e">
         <x:f>'Rental Model'!C4</x:f>
@@ -5133,7 +5149,7 @@
     <x:row r="24" spans="1:15" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A24" s="357" t="s"/>
       <x:c r="B24" s="244" t="s">
-        <x:v>70</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="C24" s="284" t="s"/>
       <x:c r="D24" s="358" t="s"/>
@@ -5144,7 +5160,7 @@
       <x:c r="I24" s="410" t="s"/>
       <x:c r="J24" s="357" t="s"/>
       <x:c r="K24" s="413" t="s">
-        <x:v>71</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="L24" s="414" t="e">
         <x:f>'Rental Model'!H7</x:f>
@@ -5154,7 +5170,7 @@
     <x:row r="25" spans="1:15" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A25" s="357" t="s"/>
       <x:c r="B25" s="359" t="s">
-        <x:v>72</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="C25" s="415" t="n">
         <x:v>0.05</x:v>
@@ -5173,7 +5189,7 @@
     <x:row r="26" spans="1:15" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A26" s="357" t="s"/>
       <x:c r="B26" s="387" t="s">
-        <x:v>73</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="C26" s="416" t="n">
         <x:v>0.3</x:v>
@@ -5186,7 +5202,7 @@
       <x:c r="I26" s="410" t="s"/>
       <x:c r="J26" s="357" t="s"/>
       <x:c r="K26" s="417" t="s">
-        <x:v>74</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="L26" s="418" t="e">
         <x:f>Tables!H29-Tables!H22</x:f>
@@ -5211,7 +5227,7 @@
     <x:row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <x:c r="A28" s="357" t="s"/>
       <x:c r="B28" s="404" t="s">
-        <x:v>75</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="C28" s="420" t="s"/>
       <x:c r="D28" s="358" t="s"/>
@@ -5227,7 +5243,7 @@
     <x:row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <x:c r="A29" s="357" t="s"/>
       <x:c r="B29" s="244" t="s">
-        <x:v>76</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="C29" s="281" t="s"/>
       <x:c r="D29" s="358" t="s"/>
@@ -5244,7 +5260,7 @@
     <x:row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <x:c r="A30" s="357" t="s"/>
       <x:c r="B30" s="243" t="s">
-        <x:v>77</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="C30" s="287" t="s"/>
       <x:c r="D30" s="358" t="s"/>
@@ -5261,7 +5277,7 @@
     <x:row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <x:c r="A31" s="357" t="s"/>
       <x:c r="B31" s="244" t="s">
-        <x:v>78</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="C31" s="281" t="s"/>
       <x:c r="D31" s="358" t="s"/>
@@ -5278,7 +5294,7 @@
     <x:row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <x:c r="A32" s="357" t="s"/>
       <x:c r="B32" s="244" t="s">
-        <x:v>79</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="C32" s="288" t="s"/>
       <x:c r="D32" s="358" t="s"/>
@@ -5295,7 +5311,7 @@
     <x:row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <x:c r="A33" s="357" t="s"/>
       <x:c r="B33" s="244" t="s">
-        <x:v>80</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="C33" s="281" t="s"/>
       <x:c r="D33" s="358" t="s"/>
@@ -5312,7 +5328,7 @@
     <x:row r="34" spans="1:15" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A34" s="357" t="s"/>
       <x:c r="B34" s="422" t="s">
-        <x:v>81</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="C34" s="423" t="s"/>
       <x:c r="D34" s="357" t="s"/>
@@ -5508,7 +5524,7 @@
       <x:c r="F2" s="439" t="s"/>
       <x:c r="G2" s="430" t="s"/>
       <x:c r="H2" s="440" t="s">
-        <x:v>82</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="I2" s="430" t="s"/>
     </x:row>
@@ -5536,52 +5552,52 @@
     <x:row r="4" spans="1:12" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A4" s="430" t="s"/>
       <x:c r="B4" s="447" t="s">
-        <x:v>83</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="C4" s="448" t="s"/>
       <x:c r="D4" s="433" t="s"/>
       <x:c r="E4" s="447" t="s">
-        <x:v>84</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="F4" s="448" t="s"/>
       <x:c r="G4" s="449" t="s"/>
       <x:c r="H4" s="450" t="s">
-        <x:v>85</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="I4" s="430" t="s"/>
     </x:row>
     <x:row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <x:c r="A5" s="430" t="s"/>
       <x:c r="B5" s="451" t="s">
-        <x:v>86</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="C5" s="452" t="e">
         <x:f>SUM(Tables!K6:K8)</x:f>
       </x:c>
       <x:c r="D5" s="433" t="s"/>
       <x:c r="E5" s="451" t="s">
-        <x:v>87</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="F5" s="453">
         <x:f>Tables!O6</x:f>
       </x:c>
       <x:c r="G5" s="449" t="s"/>
       <x:c r="H5" s="454" t="s">
-        <x:v>88</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="I5" s="430" t="s"/>
     </x:row>
     <x:row r="6" spans="1:12" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A6" s="430" t="s"/>
       <x:c r="B6" s="431" t="s">
-        <x:v>89</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="C6" s="455">
         <x:f>SUM(Tables!K9:K16)</x:f>
       </x:c>
       <x:c r="D6" s="433" t="s"/>
       <x:c r="E6" s="431" t="s">
-        <x:v>90</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="F6" s="434">
         <x:f>Tables!O7</x:f>
@@ -5595,35 +5611,35 @@
     <x:row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <x:c r="A7" s="430" t="s"/>
       <x:c r="B7" s="431" t="s">
-        <x:v>48</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="C7" s="455">
         <x:f>SUM(Tables!K18:K22)</x:f>
       </x:c>
       <x:c r="D7" s="433" t="s"/>
       <x:c r="E7" s="431" t="s">
-        <x:v>91</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="F7" s="434">
         <x:f>Tables!O8</x:f>
       </x:c>
       <x:c r="G7" s="449" t="s"/>
       <x:c r="H7" s="454" t="s">
-        <x:v>92</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="I7" s="430" t="s"/>
     </x:row>
     <x:row r="8" spans="1:12" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A8" s="430" t="s"/>
       <x:c r="B8" s="431" t="s">
-        <x:v>93</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="C8" s="455" t="e">
         <x:f>SUM(Tables!K24:K26)</x:f>
       </x:c>
       <x:c r="D8" s="433" t="s"/>
       <x:c r="E8" s="431" t="s">
-        <x:v>93</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="F8" s="434" t="e">
         <x:f>SUM(Tables!O9:O11)</x:f>
@@ -5637,7 +5653,7 @@
     <x:row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <x:c r="A9" s="430" t="s"/>
       <x:c r="B9" s="431" t="s">
-        <x:v>94</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="C9" s="455">
         <x:f>SUM(Tables!K28:K29)</x:f>
@@ -5653,7 +5669,7 @@
     <x:row r="10" spans="1:12" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A10" s="430" t="s"/>
       <x:c r="B10" s="431" t="s">
-        <x:v>95</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="C10" s="455">
         <x:f>SUM(Tables!K31:K33)</x:f>
@@ -5668,14 +5684,14 @@
     <x:row r="11" spans="1:12" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A11" s="430" t="s"/>
       <x:c r="B11" s="461" t="s">
-        <x:v>96</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="C11" s="462" t="e">
         <x:f>SUM(C5:C10)</x:f>
       </x:c>
       <x:c r="D11" s="433" t="s"/>
       <x:c r="E11" s="463" t="s">
-        <x:v>97</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="F11" s="464" t="e">
         <x:f>F5-SUM(F6:F10)-C11</x:f>
@@ -5730,7 +5746,7 @@
       <x:c r="F15" s="439" t="s"/>
       <x:c r="G15" s="430" t="s"/>
       <x:c r="H15" s="468" t="s">
-        <x:v>82</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="I15" s="430" t="s"/>
     </x:row>
@@ -5758,52 +5774,52 @@
     <x:row r="17" spans="1:12" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A17" s="430" t="s"/>
       <x:c r="B17" s="470" t="s">
-        <x:v>83</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="C17" s="471" t="s"/>
       <x:c r="D17" s="433" t="s"/>
       <x:c r="E17" s="470" t="s">
-        <x:v>84</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="F17" s="471" t="s"/>
       <x:c r="G17" s="435" t="s"/>
       <x:c r="H17" s="472" t="s">
-        <x:v>98</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="I17" s="430" t="s"/>
     </x:row>
     <x:row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <x:c r="A18" s="430" t="s"/>
       <x:c r="B18" s="451" t="s">
-        <x:v>99</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="C18" s="473" t="e">
         <x:f>SUM(Tables!K6:K8)</x:f>
       </x:c>
       <x:c r="D18" s="433" t="s"/>
       <x:c r="E18" s="451" t="s">
-        <x:v>87</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="F18" s="453">
         <x:f>Tables!O6</x:f>
       </x:c>
       <x:c r="G18" s="435" t="s"/>
       <x:c r="H18" s="454" t="s">
-        <x:v>100</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="I18" s="430" t="s"/>
     </x:row>
     <x:row r="19" spans="1:12" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A19" s="430" t="s"/>
       <x:c r="B19" s="431" t="s">
-        <x:v>101</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="C19" s="432">
         <x:f>SUM(Tables!K9:K16)</x:f>
       </x:c>
       <x:c r="D19" s="433" t="s"/>
       <x:c r="E19" s="431" t="s">
-        <x:v>90</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="F19" s="434">
         <x:f>Tables!O7</x:f>
@@ -5817,35 +5833,35 @@
     <x:row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <x:c r="A20" s="430" t="s"/>
       <x:c r="B20" s="431" t="s">
-        <x:v>48</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="C20" s="432">
         <x:f>SUM(Tables!K18:K22)</x:f>
       </x:c>
       <x:c r="D20" s="433" t="s"/>
       <x:c r="E20" s="431" t="s">
-        <x:v>91</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="F20" s="434">
         <x:f>Tables!O8</x:f>
       </x:c>
       <x:c r="G20" s="435" t="s"/>
       <x:c r="H20" s="454" t="s">
-        <x:v>102</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="I20" s="430" t="s"/>
     </x:row>
     <x:row r="21" spans="1:12" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A21" s="430" t="s"/>
       <x:c r="B21" s="431" t="s">
-        <x:v>93</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="C21" s="474" t="e">
         <x:f>SUM(Tables!K24:K26)</x:f>
       </x:c>
       <x:c r="D21" s="433" t="s"/>
       <x:c r="E21" s="431" t="s">
-        <x:v>93</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="F21" s="434" t="e">
         <x:f>SUM(Tables!O9:O11)</x:f>
@@ -5859,7 +5875,7 @@
     <x:row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <x:c r="A22" s="430" t="s"/>
       <x:c r="B22" s="431" t="s">
-        <x:v>94</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="C22" s="432">
         <x:f>SUM(Tables!K28:K29)</x:f>
@@ -5869,14 +5885,14 @@
       <x:c r="F22" s="434" t="s"/>
       <x:c r="G22" s="435" t="s"/>
       <x:c r="H22" s="454" t="s">
-        <x:v>88</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="I22" s="430" t="s"/>
     </x:row>
     <x:row r="23" spans="1:12" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A23" s="430" t="s"/>
       <x:c r="B23" s="431" t="s">
-        <x:v>95</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="C23" s="432">
         <x:f>SUM(Tables!K31:K33)</x:f>
@@ -5893,7 +5909,7 @@
     <x:row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <x:c r="A24" s="430" t="s"/>
       <x:c r="B24" s="431" t="s">
-        <x:v>103</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="C24" s="432" t="e">
         <x:f>SUM(Tables!O19:O21)</x:f>
@@ -5903,14 +5919,14 @@
       <x:c r="F24" s="434" t="s"/>
       <x:c r="G24" s="449" t="s"/>
       <x:c r="H24" s="454" t="s">
-        <x:v>92</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="I24" s="430" t="s"/>
     </x:row>
     <x:row r="25" spans="1:12" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A25" s="430" t="s"/>
       <x:c r="B25" s="431" t="s">
-        <x:v>104</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="C25" s="432">
         <x:f>Tables!O22</x:f>
@@ -5927,14 +5943,14 @@
     <x:row r="26" spans="1:12" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A26" s="430" t="s"/>
       <x:c r="B26" s="461" t="s">
-        <x:v>96</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="C26" s="478" t="e">
         <x:f>SUM(C18:C25)</x:f>
       </x:c>
       <x:c r="D26" s="433" t="s"/>
       <x:c r="E26" s="461" t="s">
-        <x:v>97</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="F26" s="479" t="e">
         <x:f>F18-SUM(F19:F25)-C26</x:f>
@@ -6013,31 +6029,31 @@
     <x:row r="32" spans="1:12" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A32" s="430" t="s"/>
       <x:c r="B32" s="484" t="s">
-        <x:v>83</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="C32" s="485" t="s"/>
       <x:c r="D32" s="433" t="s"/>
       <x:c r="E32" s="484" t="s">
-        <x:v>105</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="F32" s="485" t="s"/>
       <x:c r="G32" s="449" t="s"/>
       <x:c r="H32" s="486" t="s">
-        <x:v>106</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="I32" s="430" t="s"/>
     </x:row>
     <x:row r="33" spans="1:12" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A33" s="430" t="s"/>
       <x:c r="B33" s="487" t="s">
-        <x:v>107</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="C33" s="488" t="e">
         <x:f>SUM(Tables!K6:K22)</x:f>
       </x:c>
       <x:c r="D33" s="433" t="s"/>
       <x:c r="E33" s="487" t="s">
-        <x:v>87</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="F33" s="489" t="e">
         <x:f>Tables!D23</x:f>
@@ -6062,52 +6078,52 @@
     <x:row r="35" spans="1:12" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A35" s="430" t="s"/>
       <x:c r="B35" s="484" t="s">
-        <x:v>83</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="C35" s="485" t="s"/>
       <x:c r="D35" s="433" t="s"/>
       <x:c r="E35" s="484" t="s">
-        <x:v>84</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="F35" s="485" t="s"/>
       <x:c r="G35" s="449" t="s"/>
       <x:c r="H35" s="486" t="s">
-        <x:v>108</x:v>
+        <x:v>109</x:v>
       </x:c>
       <x:c r="I35" s="430" t="s"/>
     </x:row>
     <x:row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <x:c r="A36" s="430" t="s"/>
       <x:c r="B36" s="451" t="s">
-        <x:v>99</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="C36" s="473" t="e">
         <x:f>F33</x:f>
       </x:c>
       <x:c r="D36" s="433" t="s"/>
       <x:c r="E36" s="451" t="s">
-        <x:v>87</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="F36" s="453">
         <x:f>Tables!O6</x:f>
       </x:c>
       <x:c r="G36" s="449" t="s"/>
       <x:c r="H36" s="454" t="s">
-        <x:v>88</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="I36" s="430" t="s"/>
     </x:row>
     <x:row r="37" spans="1:12" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A37" s="430" t="s"/>
       <x:c r="B37" s="431" t="s">
-        <x:v>93</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="C37" s="432" t="e">
         <x:f>SUM(Tables!K24:K26)</x:f>
       </x:c>
       <x:c r="D37" s="433" t="s"/>
       <x:c r="E37" s="431" t="s">
-        <x:v>90</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="F37" s="434">
         <x:f>Tables!O7</x:f>
@@ -6121,35 +6137,35 @@
     <x:row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <x:c r="A38" s="430" t="s"/>
       <x:c r="B38" s="431" t="s">
-        <x:v>94</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="C38" s="432">
         <x:f>SUM(Tables!K28:K29)</x:f>
       </x:c>
       <x:c r="D38" s="433" t="s"/>
       <x:c r="E38" s="431" t="s">
-        <x:v>91</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="F38" s="434">
         <x:f>Tables!O8</x:f>
       </x:c>
       <x:c r="G38" s="449" t="s"/>
       <x:c r="H38" s="454" t="s">
-        <x:v>92</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="I38" s="430" t="s"/>
     </x:row>
     <x:row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <x:c r="A39" s="430" t="s"/>
       <x:c r="B39" s="431" t="s">
-        <x:v>95</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="C39" s="432">
         <x:f>SUM(Tables!K31:K33)</x:f>
       </x:c>
       <x:c r="D39" s="433" t="s"/>
       <x:c r="E39" s="431" t="s">
-        <x:v>93</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="F39" s="434" t="e">
         <x:f>SUM(Tables!O9:O11)</x:f>
@@ -6163,14 +6179,14 @@
     <x:row r="40" spans="1:12" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A40" s="430" t="s"/>
       <x:c r="B40" s="461" t="s">
-        <x:v>96</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="C40" s="478" t="e">
         <x:f>SUM(C36:C39)</x:f>
       </x:c>
       <x:c r="D40" s="433" t="s"/>
       <x:c r="E40" s="461" t="s">
-        <x:v>97</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="F40" s="479" t="e">
         <x:f>F36-SUM(F38:F39)-C40</x:f>
@@ -6260,25 +6276,25 @@
       <x:c r="I1" s="430" t="s"/>
       <x:c r="J1" s="357" t="s"/>
       <x:c r="K1" s="357" t="s">
-        <x:v>109</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="L1" s="357" t="s">
-        <x:v>110</x:v>
+        <x:v>111</x:v>
       </x:c>
       <x:c r="M1" s="362" t="s">
-        <x:v>111</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="N1" s="362" t="s">
-        <x:v>112</x:v>
+        <x:v>113</x:v>
       </x:c>
       <x:c r="O1" s="492" t="s">
-        <x:v>92</x:v>
+        <x:v>93</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <x:c r="A2" s="430" t="s"/>
       <x:c r="B2" s="493" t="s">
-        <x:v>113</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="C2" s="438">
         <x:f>'Data Input'!C3</x:f>
@@ -6288,7 +6304,7 @@
       <x:c r="F2" s="439" t="s"/>
       <x:c r="G2" s="430" t="s"/>
       <x:c r="H2" s="494" t="s">
-        <x:v>67</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="I2" s="430" t="s"/>
       <x:c r="J2" s="357" t="s"/>
@@ -6308,14 +6324,14 @@
     <x:row r="3" spans="1:15" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A3" s="430" t="s"/>
       <x:c r="B3" s="495" t="s">
-        <x:v>114</x:v>
+        <x:v>115</x:v>
       </x:c>
       <x:c r="C3" s="436">
         <x:f>'Data Input'!C32</x:f>
       </x:c>
       <x:c r="D3" s="436" t="s"/>
       <x:c r="E3" s="430" t="s">
-        <x:v>115</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="F3" s="496" t="n">
         <x:v>0.16</x:v>
@@ -6345,21 +6361,21 @@
     <x:row r="4" spans="1:15" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A4" s="430" t="s"/>
       <x:c r="B4" s="497" t="s">
-        <x:v>116</x:v>
+        <x:v>117</x:v>
       </x:c>
       <x:c r="C4" s="442" t="e">
         <x:f>IF('Data Input'!C34="",MATCH(1,INDEX(--(O2:O97&gt;F4),0),0),'Data Input'!C34)</x:f>
       </x:c>
       <x:c r="D4" s="442" t="s"/>
       <x:c r="E4" s="443" t="s">
-        <x:v>117</x:v>
+        <x:v>118</x:v>
       </x:c>
       <x:c r="F4" s="498" t="n">
         <x:v>0.18</x:v>
       </x:c>
       <x:c r="G4" s="430" t="s"/>
       <x:c r="H4" s="499" t="s">
-        <x:v>118</x:v>
+        <x:v>119</x:v>
       </x:c>
       <x:c r="I4" s="430" t="s"/>
       <x:c r="J4" s="357" t="s"/>
@@ -6382,12 +6398,12 @@
     <x:row r="5" spans="1:15" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A5" s="430" t="s"/>
       <x:c r="B5" s="500" t="s">
-        <x:v>119</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="C5" s="501" t="s"/>
       <x:c r="D5" s="430" t="s"/>
       <x:c r="E5" s="502" t="s">
-        <x:v>120</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="F5" s="503" t="s"/>
       <x:c r="G5" s="430" t="s"/>
@@ -6415,21 +6431,21 @@
     <x:row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <x:c r="A6" s="430" t="s"/>
       <x:c r="B6" s="505" t="s">
-        <x:v>121</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="C6" s="435">
         <x:f>'Data Input'!C29</x:f>
       </x:c>
       <x:c r="D6" s="449" t="s"/>
       <x:c r="E6" s="431" t="s">
-        <x:v>112</x:v>
+        <x:v>113</x:v>
       </x:c>
       <x:c r="F6" s="435">
         <x:f>'Data Input'!C33</x:f>
       </x:c>
       <x:c r="G6" s="430" t="s"/>
       <x:c r="H6" s="506" t="s">
-        <x:v>71</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="I6" s="430" t="s"/>
       <x:c r="J6" s="357" t="s"/>
@@ -6452,14 +6468,14 @@
     <x:row r="7" spans="1:15" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A7" s="430" t="s"/>
       <x:c r="B7" s="507" t="s">
-        <x:v>122</x:v>
+        <x:v>123</x:v>
       </x:c>
       <x:c r="C7" s="435">
         <x:f>'Data Input'!C31</x:f>
       </x:c>
       <x:c r="D7" s="449" t="s"/>
       <x:c r="E7" s="431" t="s">
-        <x:v>123</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="F7" s="435">
         <x:f>F6*0.1</x:f>
@@ -6489,21 +6505,21 @@
     <x:row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <x:c r="A8" s="430" t="s"/>
       <x:c r="B8" s="431" t="s">
-        <x:v>57</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="C8" s="435">
         <x:f>'Data Input'!C18</x:f>
       </x:c>
       <x:c r="D8" s="449" t="s"/>
       <x:c r="E8" s="431" t="s">
-        <x:v>124</x:v>
+        <x:v>125</x:v>
       </x:c>
       <x:c r="F8" s="435" t="n">
         <x:v>85</x:v>
       </x:c>
       <x:c r="G8" s="430" t="s"/>
       <x:c r="H8" s="494" t="s">
-        <x:v>125</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="I8" s="430" t="s"/>
       <x:c r="J8" s="357" t="s"/>
@@ -6526,14 +6542,14 @@
     <x:row r="9" spans="1:15" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A9" s="430" t="s"/>
       <x:c r="B9" s="431" t="s">
-        <x:v>126</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="C9" s="435">
         <x:f>SUM(C6:C8)</x:f>
       </x:c>
       <x:c r="D9" s="449" t="s"/>
       <x:c r="E9" s="431" t="s">
-        <x:v>127</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="F9" s="435">
         <x:f>50+((C3-1)*25)</x:f>
@@ -6563,21 +6579,21 @@
     <x:row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <x:c r="A10" s="430" t="s"/>
       <x:c r="B10" s="431" t="s">
-        <x:v>115</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="C10" s="435">
         <x:f>-SUM(M2:M61)</x:f>
       </x:c>
       <x:c r="D10" s="430" t="s"/>
       <x:c r="E10" s="431" t="s">
-        <x:v>128</x:v>
+        <x:v>129</x:v>
       </x:c>
       <x:c r="F10" s="435">
         <x:f>75*C3</x:f>
       </x:c>
       <x:c r="G10" s="430" t="s"/>
       <x:c r="H10" s="494" t="s">
-        <x:v>129</x:v>
+        <x:v>130</x:v>
       </x:c>
       <x:c r="I10" s="430" t="s"/>
       <x:c r="J10" s="357" t="s"/>
@@ -6600,14 +6616,14 @@
     <x:row r="11" spans="1:15" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A11" s="430" t="s"/>
       <x:c r="B11" s="510" t="s">
-        <x:v>107</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="C11" s="479">
         <x:f>C9+C10</x:f>
       </x:c>
       <x:c r="D11" s="449" t="s"/>
       <x:c r="E11" s="510" t="s">
-        <x:v>130</x:v>
+        <x:v>131</x:v>
       </x:c>
       <x:c r="F11" s="479">
         <x:f>F6-SUM(F7:F10)</x:f>
@@ -8261,10 +8277,10 @@
   <x:sheetData>
     <x:row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <x:c r="A1" s="520" t="s">
-        <x:v>131</x:v>
+        <x:v>132</x:v>
       </x:c>
       <x:c r="C1" s="521" t="s">
-        <x:v>132</x:v>
+        <x:v>133</x:v>
       </x:c>
       <x:c r="D1" s="522" t="s"/>
       <x:c r="E1" s="523" t="s"/>
@@ -8281,7 +8297,7 @@
       <x:c r="M1" s="345" t="s"/>
       <x:c r="N1" s="345" t="s"/>
       <x:c r="O1" s="136" t="s">
-        <x:v>133</x:v>
+        <x:v>134</x:v>
       </x:c>
       <x:c r="P1" s="165">
         <x:f>'Data Input'!C24</x:f>
@@ -8292,14 +8308,14 @@
     <x:row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <x:c r="A2" s="527" t="s"/>
       <x:c r="C2" s="9" t="s">
-        <x:v>99</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="D2" s="528" t="s">
-        <x:v>134</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="E2" s="528" t="s"/>
       <x:c r="F2" s="529" t="s">
-        <x:v>135</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="G2" s="529" t="s"/>
       <x:c r="H2" s="10" t="s"/>
@@ -8315,7 +8331,7 @@
       </x:c>
       <x:c r="N2" s="533" t="s"/>
       <x:c r="O2" s="534" t="s">
-        <x:v>136</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="P2" s="535">
         <x:f>'Data Input'!C26</x:f>
@@ -8325,7 +8341,7 @@
     </x:row>
     <x:row r="3" spans="1:21" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A3" s="536" t="s">
-        <x:v>137</x:v>
+        <x:v>138</x:v>
       </x:c>
       <x:c r="C3" s="11" t="e">
         <x:f>Tables!K6</x:f>
@@ -8340,7 +8356,7 @@
       <x:c r="G3" s="537" t="s"/>
       <x:c r="H3" s="10" t="s"/>
       <x:c r="J3" s="51" t="s">
-        <x:v>138</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="K3" s="141">
         <x:f>'Data Input'!C10</x:f>
@@ -8353,7 +8369,7 @@
         <x:f>'Data Input'!C12</x:f>
       </x:c>
       <x:c r="O3" s="143" t="s">
-        <x:v>139</x:v>
+        <x:v>140</x:v>
       </x:c>
       <x:c r="P3" s="169" t="n">
         <x:v>0</x:v>
@@ -8363,7 +8379,7 @@
     </x:row>
     <x:row r="4" spans="1:21" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A4" s="538" t="s">
-        <x:v>140</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="C4" s="12" t="s"/>
       <x:c r="D4" s="355" t="s"/>
@@ -8375,45 +8391,45 @@
     </x:row>
     <x:row r="5" spans="1:21" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A5" s="538" t="s">
-        <x:v>141</x:v>
+        <x:v>142</x:v>
       </x:c>
       <x:c r="C5" s="14" t="s">
-        <x:v>142</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="D5" s="539" t="s">
-        <x:v>143</x:v>
+        <x:v>144</x:v>
       </x:c>
       <x:c r="E5" s="539" t="s">
-        <x:v>144</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="F5" s="539" t="s">
-        <x:v>145</x:v>
+        <x:v>146</x:v>
       </x:c>
       <x:c r="G5" s="539" t="s">
-        <x:v>146</x:v>
+        <x:v>147</x:v>
       </x:c>
       <x:c r="H5" s="16" t="s">
-        <x:v>147</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="J5" s="540" t="s">
-        <x:v>148</x:v>
+        <x:v>149</x:v>
       </x:c>
       <x:c r="K5" s="541" t="s"/>
       <x:c r="L5" s="542" t="s">
-        <x:v>149</x:v>
+        <x:v>150</x:v>
       </x:c>
       <x:c r="N5" s="540" t="s">
-        <x:v>150</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="O5" s="541" t="s"/>
       <x:c r="Q5" s="360" t="s">
-        <x:v>151</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="R5" s="361" t="s"/>
     </x:row>
     <x:row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <x:c r="A6" s="538" t="s">
-        <x:v>152</x:v>
+        <x:v>153</x:v>
       </x:c>
       <x:c r="C6" s="17" t="n">
         <x:v>35001</x:v>
@@ -8434,7 +8450,7 @@
         <x:f>((D6-C6)*F6)+344</x:f>
       </x:c>
       <x:c r="J6" s="127" t="s">
-        <x:v>86</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="K6" s="145" t="e">
         <x:f>(O6-SUM(K7:K16,K18:K22,K25:K26,K28:K29,K31:K33,O7:O11)-(SUM(K7:K16,K18:K22,K25:K26,K28:K29,K31:K33)*P2))/((P2*1.0058)+1.0058)</x:f>
@@ -8443,13 +8459,13 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="N6" s="127" t="s">
-        <x:v>153</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="O6" s="145">
         <x:f>'Data Input'!C22</x:f>
       </x:c>
       <x:c r="Q6" s="545" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="R6" s="546" t="e">
         <x:f>'Flip Sheets'!C11</x:f>
@@ -8457,7 +8473,7 @@
     </x:row>
     <x:row r="7" spans="1:21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="A7" s="538" t="s">
-        <x:v>154</x:v>
+        <x:v>155</x:v>
       </x:c>
       <x:c r="C7" s="17" t="n">
         <x:v>50001</x:v>
@@ -8478,7 +8494,7 @@
         <x:f>((D7-C7)*F7)+H6</x:f>
       </x:c>
       <x:c r="J7" s="127" t="s">
-        <x:v>155</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="K7" s="145">
         <x:f>'Data Input'!I3*(1+(L7*'Data Input'!C24))</x:f>
@@ -8487,13 +8503,13 @@
         <x:f>0.09/12</x:f>
       </x:c>
       <x:c r="N7" s="127" t="s">
-        <x:v>90</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="O7" s="145" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="Q7" s="548" t="s">
-        <x:v>156</x:v>
+        <x:v>157</x:v>
       </x:c>
       <x:c r="R7" s="549" t="e">
         <x:f>'Flip Sheets'!F11</x:f>
@@ -8501,7 +8517,7 @@
     </x:row>
     <x:row r="8" spans="1:21" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A8" s="550" t="s">
-        <x:v>157</x:v>
+        <x:v>158</x:v>
       </x:c>
       <x:c r="C8" s="17" t="n">
         <x:v>100001</x:v>
@@ -8522,7 +8538,7 @@
         <x:f>((D8-C8)*F8)+H7</x:f>
       </x:c>
       <x:c r="J8" s="551" t="s">
-        <x:v>158</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="K8" s="145">
         <x:f>'Data Input'!I4*L8</x:f>
@@ -8531,13 +8547,13 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="N8" s="127" t="s">
-        <x:v>91</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="O8" s="145">
         <x:f>O6*'Data Input'!C25</x:f>
       </x:c>
       <x:c r="Q8" s="548" t="s">
-        <x:v>159</x:v>
+        <x:v>160</x:v>
       </x:c>
       <x:c r="R8" s="552" t="e">
         <x:f>'Flip Sheets'!H8</x:f>
@@ -8564,7 +8580,7 @@
         <x:f>((D9-C9)*F9)+H8</x:f>
       </x:c>
       <x:c r="J9" s="127" t="s">
-        <x:v>160</x:v>
+        <x:v>161</x:v>
       </x:c>
       <x:c r="K9" s="145">
         <x:f>'Data Input'!I5*L9</x:f>
@@ -8573,13 +8589,13 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="N9" s="127" t="s">
-        <x:v>161</x:v>
+        <x:v>162</x:v>
       </x:c>
       <x:c r="O9" s="145" t="e">
         <x:f>(IF('Data Input'!C2="Residential",IF(AND(O6&gt;0,O6&lt;=500000),"1%",IF(O6&gt;500000,"1.425%","")),IF(AND(O6&gt;0,O6&lt;=500000),"1.425%",IF(O6&gt;500000,"2.625%","")))+0.4%)*O6</x:f>
       </x:c>
       <x:c r="Q9" s="553" t="s">
-        <x:v>162</x:v>
+        <x:v>163</x:v>
       </x:c>
       <x:c r="R9" s="554" t="e">
         <x:f>R8/'Data Input'!C24*12</x:f>
@@ -8587,7 +8603,7 @@
     </x:row>
     <x:row r="10" spans="1:21" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A10" s="520" t="s">
-        <x:v>163</x:v>
+        <x:v>164</x:v>
       </x:c>
       <x:c r="C10" s="17" t="n">
         <x:v>1000001</x:v>
@@ -8608,7 +8624,7 @@
         <x:f>((D10-C10)*F10)+H9</x:f>
       </x:c>
       <x:c r="J10" s="127" t="s">
-        <x:v>164</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="K10" s="145">
         <x:f>'Data Input'!I6*L10</x:f>
@@ -8617,7 +8633,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="N10" s="127" t="s">
-        <x:v>165</x:v>
+        <x:v>166</x:v>
       </x:c>
       <x:c r="O10" s="145" t="n">
         <x:v>1250</x:v>
@@ -8646,7 +8662,7 @@
         <x:f>((D11-C11)*F11)+H10</x:f>
       </x:c>
       <x:c r="J11" s="127" t="s">
-        <x:v>166</x:v>
+        <x:v>167</x:v>
       </x:c>
       <x:c r="K11" s="145">
         <x:f>('Data Input'!I7*(1+(P1*0.0075)))*L11</x:f>
@@ -8655,19 +8671,19 @@
         <x:v>0.35</x:v>
       </x:c>
       <x:c r="N11" s="127" t="s">
-        <x:v>167</x:v>
+        <x:v>168</x:v>
       </x:c>
       <x:c r="O11" s="145" t="n">
         <x:v>500</x:v>
       </x:c>
       <x:c r="Q11" s="555" t="s">
-        <x:v>168</x:v>
+        <x:v>169</x:v>
       </x:c>
       <x:c r="R11" s="556" t="s"/>
     </x:row>
     <x:row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <x:c r="A12" s="536" t="s">
-        <x:v>169</x:v>
+        <x:v>170</x:v>
       </x:c>
       <x:c r="C12" s="17" t="n">
         <x:v>10000001</x:v>
@@ -8688,7 +8704,7 @@
         <x:f>((D12-C12)*F12)+H11</x:f>
       </x:c>
       <x:c r="J12" s="127" t="s">
-        <x:v>170</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="K12" s="145">
         <x:f>'Data Input'!I8*L12</x:f>
@@ -8697,11 +8713,11 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="N12" s="540" t="s">
-        <x:v>171</x:v>
+        <x:v>172</x:v>
       </x:c>
       <x:c r="O12" s="557" t="s"/>
       <x:c r="Q12" s="558" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="R12" s="559" t="e">
         <x:f>'Flip Sheets'!C26</x:f>
@@ -8709,7 +8725,7 @@
     </x:row>
     <x:row r="13" spans="1:21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="A13" s="538" t="s">
-        <x:v>172</x:v>
+        <x:v>173</x:v>
       </x:c>
       <x:c r="C13" s="17" t="n">
         <x:v>15000001</x:v>
@@ -8724,7 +8740,7 @@
       <x:c r="G13" s="512" t="s"/>
       <x:c r="H13" s="20" t="s"/>
       <x:c r="J13" s="127" t="s">
-        <x:v>173</x:v>
+        <x:v>174</x:v>
       </x:c>
       <x:c r="K13" s="145">
         <x:f>'Data Input'!I9*L13</x:f>
@@ -8733,13 +8749,13 @@
         <x:v>0.4</x:v>
       </x:c>
       <x:c r="N13" s="127" t="s">
-        <x:v>100</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="O13" s="145">
         <x:f>O6*O17</x:f>
       </x:c>
       <x:c r="Q13" s="560" t="s">
-        <x:v>174</x:v>
+        <x:v>175</x:v>
       </x:c>
       <x:c r="R13" s="561" t="e">
         <x:f>'Flip Sheets'!F26</x:f>
@@ -8747,7 +8763,7 @@
     </x:row>
     <x:row r="14" spans="1:21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="A14" s="562" t="s">
-        <x:v>175</x:v>
+        <x:v>176</x:v>
       </x:c>
       <x:c r="C14" s="12" t="s"/>
       <x:c r="D14" s="355" t="s"/>
@@ -8756,7 +8772,7 @@
       <x:c r="G14" s="355" t="s"/>
       <x:c r="H14" s="10" t="s"/>
       <x:c r="J14" s="127" t="s">
-        <x:v>176</x:v>
+        <x:v>177</x:v>
       </x:c>
       <x:c r="K14" s="145">
         <x:f>'Data Input'!I10*L14</x:f>
@@ -8765,13 +8781,13 @@
         <x:v>0.15</x:v>
       </x:c>
       <x:c r="N14" s="127" t="s">
-        <x:v>177</x:v>
+        <x:v>178</x:v>
       </x:c>
       <x:c r="O14" s="128" t="n">
         <x:v>0.12</x:v>
       </x:c>
       <x:c r="Q14" s="560" t="s">
-        <x:v>178</x:v>
+        <x:v>179</x:v>
       </x:c>
       <x:c r="R14" s="563" t="e">
         <x:f>'Flip Sheets'!H25</x:f>
@@ -8779,24 +8795,24 @@
     </x:row>
     <x:row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <x:c r="A15" s="538" t="s">
-        <x:v>179</x:v>
+        <x:v>180</x:v>
       </x:c>
       <x:c r="C15" s="14" t="s">
-        <x:v>144</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="D15" s="528" t="s">
-        <x:v>180</x:v>
+        <x:v>181</x:v>
       </x:c>
       <x:c r="E15" s="528" t="s"/>
       <x:c r="F15" s="355" t="s"/>
       <x:c r="G15" s="564" t="s">
-        <x:v>181</x:v>
+        <x:v>182</x:v>
       </x:c>
       <x:c r="H15" s="16" t="s">
-        <x:v>182</x:v>
+        <x:v>183</x:v>
       </x:c>
       <x:c r="J15" s="127" t="s">
-        <x:v>183</x:v>
+        <x:v>184</x:v>
       </x:c>
       <x:c r="K15" s="145">
         <x:f>'Data Input'!I11*L15</x:f>
@@ -8805,13 +8821,13 @@
         <x:f>IF('Data Input'!I11&lt;12500,100%,0%)</x:f>
       </x:c>
       <x:c r="N15" s="127" t="s">
-        <x:v>184</x:v>
+        <x:v>185</x:v>
       </x:c>
       <x:c r="O15" s="23" t="n">
         <x:v>2</x:v>
       </x:c>
       <x:c r="Q15" s="565" t="s">
-        <x:v>162</x:v>
+        <x:v>163</x:v>
       </x:c>
       <x:c r="R15" s="566" t="e">
         <x:f>R14/'Data Input'!C24*12</x:f>
@@ -8819,7 +8835,7 @@
     </x:row>
     <x:row r="16" spans="1:21" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A16" s="538" t="s">
-        <x:v>185</x:v>
+        <x:v>186</x:v>
       </x:c>
       <x:c r="C16" s="21" t="e">
         <x:f>IF(C3&lt;C6,402,IF(C3&lt;=D6,(C3-C6)*E6,IF(C3&lt;=D7,(C3-C7)*E7+G6,IF(C3&lt;=D8,(C3-C8)*E8+G7,IF(C3&lt;=D9,(C3-C9)*E9+G8,IF(C3&lt;=D10,(C3-C10)*E10+G9,IF(C3&lt;=D11,(C3-C11)*E11+G10,IF(C3&lt;=D12,(C3-C12)*E12+G11,IF(C3&gt;=C13,(C3-C13)*E13+G12,"")))))))))</x:f>
@@ -8838,7 +8854,7 @@
         <x:f>D16+E16+G16</x:f>
       </x:c>
       <x:c r="J16" s="130" t="s">
-        <x:v>186</x:v>
+        <x:v>187</x:v>
       </x:c>
       <x:c r="K16" s="147">
         <x:f>IF('Data Input'!I14="",0,'Data Input'!I13*(1+(TODAY()+180-'Data Input'!I14)*L16))</x:f>
@@ -8847,7 +8863,7 @@
         <x:f>9%/365</x:f>
       </x:c>
       <x:c r="N16" s="127" t="s">
-        <x:v>187</x:v>
+        <x:v>188</x:v>
       </x:c>
       <x:c r="O16" s="23" t="n">
         <x:v>12</x:v>
@@ -8861,21 +8877,21 @@
     </x:row>
     <x:row r="17" spans="1:21" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A17" s="538" t="s">
-        <x:v>188</x:v>
+        <x:v>189</x:v>
       </x:c>
       <x:c r="J17" s="517" t="s">
-        <x:v>189</x:v>
+        <x:v>190</x:v>
       </x:c>
       <x:c r="K17" s="569" t="s"/>
       <x:c r="L17" s="570" t="s"/>
       <x:c r="N17" s="127" t="s">
-        <x:v>102</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="O17" s="129" t="n">
         <x:v>0.6</x:v>
       </x:c>
       <x:c r="Q17" s="560" t="s">
-        <x:v>190</x:v>
+        <x:v>191</x:v>
       </x:c>
       <x:c r="R17" s="563" t="e">
         <x:f>R13/R16</x:f>
@@ -8883,33 +8899,33 @@
     </x:row>
     <x:row r="18" spans="1:21" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A18" s="550" t="s">
-        <x:v>191</x:v>
+        <x:v>192</x:v>
       </x:c>
       <x:c r="C18" s="521" t="s">
-        <x:v>161</x:v>
+        <x:v>162</x:v>
       </x:c>
       <x:c r="D18" s="571" t="s"/>
       <x:c r="F18" s="572" t="s"/>
       <x:c r="G18" s="573" t="s">
-        <x:v>192</x:v>
+        <x:v>193</x:v>
       </x:c>
       <x:c r="H18" s="574" t="n">
         <x:v>0.25</x:v>
       </x:c>
       <x:c r="I18" s="572" t="s"/>
       <x:c r="J18" s="127" t="s">
-        <x:v>193</x:v>
+        <x:v>194</x:v>
       </x:c>
       <x:c r="K18" s="145">
         <x:f>'Data Input'!C15</x:f>
       </x:c>
       <x:c r="L18" s="575" t="s"/>
       <x:c r="N18" s="517" t="s">
-        <x:v>194</x:v>
+        <x:v>195</x:v>
       </x:c>
       <x:c r="O18" s="576" t="s"/>
       <x:c r="Q18" s="577" t="s">
-        <x:v>195</x:v>
+        <x:v>196</x:v>
       </x:c>
       <x:c r="R18" s="578" t="e">
         <x:f>R17/'Data Input'!C24*12</x:f>
@@ -8918,21 +8934,21 @@
     <x:row r="19" spans="1:21" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A19" s="355" t="s"/>
       <x:c r="C19" s="579" t="s">
-        <x:v>196</x:v>
+        <x:v>197</x:v>
       </x:c>
       <x:c r="D19" s="56" t="str">
         <x:f>IF(OR(NOT(ISERROR(SEARCH(("A"),'Data Input'!C4))),NOT(ISERROR(SEARCH(("B"),'Data Input'!C4))),NOT(ISERROR(SEARCH(("C0"),'Data Input'!C4))),NOT(ISERROR(SEARCH(("21"),'Data Input'!C4))),NOT(ISERROR(SEARCH(("R"),'Data Input'!C4)))),"Residential","Not Residential")</x:f>
       </x:c>
       <x:c r="F19" s="514" t="s"/>
       <x:c r="G19" s="580" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="H19" s="581" t="e">
         <x:f>(Tables!O6-SUM(Tables!K24:K33,Tables!O7:O11,O19:O22)-(SUM(Tables!K24:K33,O19:O22)*Tables!H18))/((Tables!H18*1)+1)</x:f>
       </x:c>
       <x:c r="I19" s="514" t="s"/>
       <x:c r="J19" s="127" t="s">
-        <x:v>197</x:v>
+        <x:v>198</x:v>
       </x:c>
       <x:c r="K19" s="582">
         <x:f>IF(OR('Data Input'!C11="Yes",'Data Input'!C12&gt;0)*AND('Data Input'!F8&lt;&gt;"Yes",'Data Input'!F9&lt;&gt;"Yes",'Data Input'!F10&lt;&gt;"Yes",'Data Input'!C16&lt;&gt;""),'Data Input'!C16*L19-10000,'Data Input'!C16*L19)</x:f>
@@ -8941,7 +8957,7 @@
         <x:v>0.75</x:v>
       </x:c>
       <x:c r="N19" s="127" t="s">
-        <x:v>145</x:v>
+        <x:v>146</x:v>
       </x:c>
       <x:c r="O19" s="179" t="e">
         <x:f>Tables!H16-Tables!C16</x:f>
@@ -8951,38 +8967,38 @@
     </x:row>
     <x:row r="20" spans="1:21" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A20" s="584" t="s">
-        <x:v>198</x:v>
+        <x:v>199</x:v>
       </x:c>
       <x:c r="F20" s="514" t="s"/>
       <x:c r="G20" s="585" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="H20" s="586" t="e">
         <x:f>H19+SUM(K24:K33,O19:O22)</x:f>
       </x:c>
       <x:c r="I20" s="514" t="s"/>
       <x:c r="J20" s="127" t="s">
-        <x:v>55</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="K20" s="145">
         <x:f>'Data Input'!C17</x:f>
       </x:c>
       <x:c r="L20" s="575" t="s"/>
       <x:c r="N20" s="127" t="s">
-        <x:v>199</x:v>
+        <x:v>200</x:v>
       </x:c>
       <x:c r="O20" s="145" t="e">
         <x:f>((IF('Data Input'!C2="Residential",IF(AND(O13&gt;0,O13&lt;=500000),"2.0%",IF(O13&gt;500000,"2.125%","")),IF(AND(O13&gt;0,O13&lt;=500000),"2.0%",IF(O13&gt;500000,"2.75%",""))))*O13)+(275)+1500</x:f>
       </x:c>
       <x:c r="Q20" s="587" t="s">
-        <x:v>200</x:v>
+        <x:v>201</x:v>
       </x:c>
       <x:c r="R20" s="588" t="s"/>
     </x:row>
     <x:row r="21" spans="1:21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="A21" s="589" t="s"/>
       <x:c r="C21" s="384" t="s">
-        <x:v>201</x:v>
+        <x:v>202</x:v>
       </x:c>
       <x:c r="D21" s="590" t="s"/>
       <x:c r="F21" s="514" t="s"/>
@@ -8994,20 +9010,20 @@
       </x:c>
       <x:c r="I21" s="514" t="s"/>
       <x:c r="J21" s="127" t="s">
-        <x:v>202</x:v>
+        <x:v>203</x:v>
       </x:c>
       <x:c r="K21" s="145">
         <x:f>'Data Input'!C12*5000</x:f>
       </x:c>
       <x:c r="L21" s="575" t="s"/>
       <x:c r="N21" s="127" t="s">
-        <x:v>203</x:v>
+        <x:v>204</x:v>
       </x:c>
       <x:c r="O21" s="145">
         <x:f>(O13*O15%)</x:f>
       </x:c>
       <x:c r="Q21" s="591" t="s">
-        <x:v>105</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="R21" s="592" t="e">
         <x:f>'Flip Sheets'!F33</x:f>
@@ -9015,7 +9031,7 @@
     </x:row>
     <x:row r="22" spans="1:21" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A22" s="513" t="s">
-        <x:v>204</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="C22" s="53" t="s">
         <x:v>205</x:v>
@@ -9039,13 +9055,13 @@
       </x:c>
       <x:c r="L22" s="575" t="s"/>
       <x:c r="N22" s="130" t="s">
-        <x:v>104</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="O22" s="147">
         <x:f>(O13*O14/12*'Data Input'!C24)</x:f>
       </x:c>
       <x:c r="Q22" s="595" t="s">
-        <x:v>107</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="R22" s="596" t="e">
         <x:f>'Flip Sheets'!C33</x:f>
@@ -9053,10 +9069,10 @@
     </x:row>
     <x:row r="23" spans="1:21" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A23" s="597" t="s">
-        <x:v>28</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="C23" s="54" t="s">
-        <x:v>105</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="D23" s="96" t="e">
         <x:f>(Tables!O6-SUM(Tables!K24:K33,Tables!O7:O11)-(SUM(Tables!K24:K33)*Tables!D22))/((Tables!D22*1)+1)</x:f>
@@ -9070,7 +9086,7 @@
       </x:c>
       <x:c r="I23" s="514" t="s"/>
       <x:c r="J23" s="517" t="s">
-        <x:v>93</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="K23" s="518" t="s"/>
       <x:c r="L23" s="570" t="s"/>
@@ -9079,7 +9095,7 @@
       <x:c r="O23" s="598" t="s"/>
       <x:c r="P23" s="598" t="s"/>
       <x:c r="Q23" s="599" t="s">
-        <x:v>106</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="R23" s="600" t="e">
         <x:f>R21-R22</x:f>
@@ -9105,7 +9121,7 @@
     </x:row>
     <x:row r="25" spans="1:21" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A25" s="584" t="s">
-        <x:v>148</x:v>
+        <x:v>149</x:v>
       </x:c>
       <x:c r="C25" s="521" t="s">
         <x:v>208</x:v>
@@ -9132,14 +9148,14 @@
     <x:row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <x:c r="A26" s="513" t="s"/>
       <x:c r="C26" s="2" t="s">
-        <x:v>139</x:v>
+        <x:v>140</x:v>
       </x:c>
       <x:c r="D26" s="180" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="F26" s="514" t="s"/>
       <x:c r="G26" s="580" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="H26" s="581">
         <x:f>'Data Input'!C21+SUM(Tables!K9:K16,K18,K20:K22)</x:f>
@@ -9159,7 +9175,7 @@
     </x:row>
     <x:row r="27" spans="1:21" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A27" s="513" t="s">
-        <x:v>28</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="C27" s="51" t="s">
         <x:v>212</x:v>
@@ -9169,7 +9185,7 @@
       </x:c>
       <x:c r="F27" s="514" t="s"/>
       <x:c r="G27" s="585" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="H27" s="586" t="e">
         <x:f>H26+SUM(K24:K33,O19:O22)</x:f>
@@ -9246,7 +9262,7 @@
       </x:c>
       <x:c r="I30" s="355" t="s"/>
       <x:c r="J30" s="517" t="s">
-        <x:v>95</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="K30" s="518" t="s"/>
       <x:c r="L30" s="519" t="s"/>
@@ -9260,7 +9276,7 @@
       <x:c r="F31" s="514" t="s"/>
       <x:c r="I31" s="355" t="s"/>
       <x:c r="J31" s="127" t="s">
-        <x:v>124</x:v>
+        <x:v>125</x:v>
       </x:c>
       <x:c r="K31" s="145">
         <x:f>(O13/100)*0.45/12*P1</x:f>

</xml_diff>

<commit_message>
fixed a but that underwriter's update message that not showing up
</commit_message>
<xml_diff>
--- a/IntranetPortal/IntranetPortal/TempDataFile/underwriter.xlsx
+++ b/IntranetPortal/IntranetPortal/TempDataFile/underwriter.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="223">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="225">
   <x:si>
     <x:t>Property Info</x:t>
   </x:si>
@@ -56,7 +56,7 @@
     <x:t>Property Address:</x:t>
   </x:si>
   <x:si>
-    <x:t>122-14 134 ST, SOUTH OZONE PARK,NY 11420</x:t>
+    <x:t>112-44 180 ST, ST. ALBANS,NY 11433</x:t>
   </x:si>
   <x:si>
     <x:t>1st Mortgage</x:t>
@@ -80,7 +80,7 @@
     <x:t>Building Dimension</x:t>
   </x:si>
   <x:si>
-    <x:t>24'x50'</x:t>
+    <x:t>21.5'x33.42'</x:t>
   </x:si>
   <x:si>
     <x:t>COS Recorded:</x:t>
@@ -110,7 +110,7 @@
     <x:t>Zoning</x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">R3-2     </x:t>
+    <x:t xml:space="preserve">R2       </x:t>
   </x:si>
   <x:si>
     <x:t>Other Liens:</x:t>
@@ -140,6 +140,9 @@
     <x:t>Fannie Mae:</x:t>
   </x:si>
   <x:si>
+    <x:t>Yes</x:t>
+  </x:si>
+  <x:si>
     <x:t>Personal Judgements:</x:t>
   </x:si>
   <x:si>
@@ -164,6 +167,9 @@
     <x:t>Servicer:</x:t>
   </x:si>
   <x:si>
+    <x:t>golden rush</x:t>
+  </x:si>
+  <x:si>
     <x:t>IRS/NYS Tax Liens:</x:t>
   </x:si>
   <x:si>
@@ -173,10 +179,10 @@
     <x:t>Foreclosure Index #:</x:t>
   </x:si>
   <x:si>
+    <x:t>2425/25222</x:t>
+  </x:si>
+  <x:si>
     <x:t>Vacate Order:</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Yes</x:t>
   </x:si>
   <x:si>
     <x:t>BEST CASE SCENARIO</x:t>
@@ -4645,7 +4651,7 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="F3" s="290" t="n">
-        <x:v>0</x:v>
+        <x:v>3500</x:v>
       </x:c>
       <x:c r="G3" s="358" t="s"/>
       <x:c r="H3" s="244" t="s">
@@ -4676,15 +4682,13 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="F4" s="290" t="n">
-        <x:v>0</x:v>
+        <x:v>200</x:v>
       </x:c>
       <x:c r="G4" s="358" t="s"/>
       <x:c r="H4" s="244" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="I4" s="281" t="n">
-        <x:v>0</x:v>
-      </x:c>
+      <x:c r="I4" s="281" t="s"/>
       <x:c r="J4" s="357" t="s"/>
       <x:c r="K4" s="357" t="s"/>
       <x:c r="L4" s="362" t="s"/>
@@ -4709,7 +4713,9 @@
       <x:c r="H5" s="244" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="I5" s="281" t="s"/>
+      <x:c r="I5" s="281" t="n">
+        <x:v>2500</x:v>
+      </x:c>
       <x:c r="J5" s="357" t="s"/>
       <x:c r="K5" s="370" t="s">
         <x:v>17</x:v>
@@ -4724,7 +4730,7 @@
         <x:v>18</x:v>
       </x:c>
       <x:c r="C6" s="274" t="n">
-        <x:v>58</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="D6" s="358" t="s"/>
       <x:c r="E6" s="244" t="s">
@@ -4737,7 +4743,9 @@
       <x:c r="H6" s="244" t="s">
         <x:v>20</x:v>
       </x:c>
-      <x:c r="I6" s="281" t="s"/>
+      <x:c r="I6" s="281" t="n">
+        <x:v>3422</x:v>
+      </x:c>
       <x:c r="J6" s="357" t="s"/>
       <x:c r="K6" s="373" t="s">
         <x:v>21</x:v>
@@ -4812,16 +4820,16 @@
         <x:v>32</x:v>
       </x:c>
       <x:c r="F9" s="279" t="s">
-        <x:v>15</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="G9" s="358" t="s"/>
       <x:c r="H9" s="244" t="s">
-        <x:v>33</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="I9" s="281" t="s"/>
       <x:c r="J9" s="357" t="s"/>
       <x:c r="K9" s="375" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="L9" s="377" t="e">
         <x:f>'Flip Sheets'!F26</x:f>
@@ -4831,24 +4839,24 @@
     <x:row r="10" spans="1:15" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A10" s="357" t="s"/>
       <x:c r="B10" s="244" t="s">
-        <x:v>35</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="C10" s="279" t="s"/>
       <x:c r="D10" s="358" t="s"/>
       <x:c r="E10" s="244" t="s">
-        <x:v>36</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="F10" s="279" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="G10" s="358" t="s"/>
       <x:c r="H10" s="244" t="s">
-        <x:v>37</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="I10" s="281" t="s"/>
       <x:c r="J10" s="357" t="s"/>
       <x:c r="K10" s="378" t="s">
-        <x:v>38</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="L10" s="379" t="e">
         <x:f>'Flip Sheets'!H25</x:f>
@@ -4858,17 +4866,19 @@
     <x:row r="11" spans="1:15" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A11" s="357" t="s"/>
       <x:c r="B11" s="243" t="s">
-        <x:v>39</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="C11" s="279" t="s"/>
       <x:c r="D11" s="358" t="s"/>
       <x:c r="E11" s="244" t="s">
-        <x:v>40</x:v>
-      </x:c>
-      <x:c r="F11" s="279" t="s"/>
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="F11" s="279" t="s">
+        <x:v>42</x:v>
+      </x:c>
       <x:c r="G11" s="358" t="s"/>
       <x:c r="H11" s="244" t="s">
-        <x:v>41</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="I11" s="281" t="n">
         <x:v>0</x:v>
@@ -4881,24 +4891,26 @@
     <x:row r="12" spans="1:15" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A12" s="357" t="s"/>
       <x:c r="B12" s="248" t="s">
-        <x:v>42</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="C12" s="280" t="s"/>
       <x:c r="D12" s="358" t="s"/>
       <x:c r="E12" s="359" t="s">
-        <x:v>43</x:v>
-      </x:c>
-      <x:c r="F12" s="274" t="s"/>
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="F12" s="274" t="s">
+        <x:v>46</x:v>
+      </x:c>
       <x:c r="G12" s="358" t="s"/>
       <x:c r="H12" s="244" t="s">
-        <x:v>44</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="I12" s="287" t="s">
-        <x:v>45</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="J12" s="357" t="s"/>
       <x:c r="K12" s="360" t="s">
-        <x:v>46</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="L12" s="361" t="s"/>
       <x:c r="M12" s="357" t="s"/>
@@ -4909,16 +4921,14 @@
       <x:c r="C13" s="358" t="s"/>
       <x:c r="D13" s="358" t="s"/>
       <x:c r="E13" s="244" t="s">
-        <x:v>47</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="F13" s="291" t="s"/>
       <x:c r="G13" s="357" t="s"/>
       <x:c r="H13" s="244" t="s">
-        <x:v>48</x:v>
-      </x:c>
-      <x:c r="I13" s="281" t="n">
-        <x:v>0</x:v>
-      </x:c>
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="I13" s="281" t="s"/>
       <x:c r="J13" s="357" t="s"/>
       <x:c r="K13" s="382" t="s">
         <x:v>21</x:v>
@@ -4931,17 +4941,17 @@
     <x:row r="14" spans="1:15" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A14" s="357" t="s"/>
       <x:c r="B14" s="384" t="s">
-        <x:v>49</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="C14" s="385" t="s"/>
       <x:c r="D14" s="386" t="s"/>
       <x:c r="E14" s="244" t="s">
-        <x:v>50</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="F14" s="275" t="s"/>
       <x:c r="G14" s="358" t="s"/>
       <x:c r="H14" s="387" t="s">
-        <x:v>51</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="I14" s="388" t="s"/>
       <x:c r="J14" s="357" t="s"/>
@@ -4956,12 +4966,12 @@
     <x:row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <x:c r="A15" s="357" t="s"/>
       <x:c r="B15" s="244" t="s">
-        <x:v>52</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="C15" s="281" t="s"/>
       <x:c r="D15" s="386" t="s"/>
       <x:c r="E15" s="243" t="s">
-        <x:v>53</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="F15" s="391" t="s"/>
       <x:c r="G15" s="358" t="s"/>
@@ -4979,12 +4989,12 @@
     <x:row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <x:c r="A16" s="357" t="s"/>
       <x:c r="B16" s="244" t="s">
-        <x:v>54</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="C16" s="281" t="s"/>
       <x:c r="D16" s="357" t="s"/>
       <x:c r="E16" s="244" t="s">
-        <x:v>55</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="F16" s="294" t="s"/>
       <x:c r="G16" s="358" t="s"/>
@@ -4992,7 +5002,7 @@
       <x:c r="I16" s="392" t="s"/>
       <x:c r="J16" s="357" t="s"/>
       <x:c r="K16" s="389" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="L16" s="393" t="e">
         <x:f>('Flip Sheets'!$F$18-SUM('Flip Sheets'!$F$19:$F$25)-(L13+SUM('Flip Sheets'!$C$21:$C$25)))</x:f>
@@ -5002,12 +5012,12 @@
     <x:row r="17" spans="1:15" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A17" s="357" t="s"/>
       <x:c r="B17" s="243" t="s">
-        <x:v>56</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="C17" s="394" t="s"/>
       <x:c r="D17" s="386" t="s"/>
       <x:c r="E17" s="244" t="s">
-        <x:v>57</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="F17" s="278" t="s"/>
       <x:c r="G17" s="358" t="s"/>
@@ -5015,7 +5025,7 @@
       <x:c r="I17" s="392" t="s"/>
       <x:c r="J17" s="357" t="s"/>
       <x:c r="K17" s="395" t="s">
-        <x:v>38</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="L17" s="396" t="e">
         <x:f>L16/L14</x:f>
@@ -5025,12 +5035,12 @@
     <x:row r="18" spans="1:15" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A18" s="357" t="s"/>
       <x:c r="B18" s="397" t="s">
-        <x:v>58</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="C18" s="283" t="s"/>
       <x:c r="D18" s="358" t="s"/>
       <x:c r="E18" s="244" t="s">
-        <x:v>59</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="F18" s="294" t="s"/>
       <x:c r="G18" s="357" t="s"/>
@@ -5047,7 +5057,7 @@
       <x:c r="C19" s="398" t="s"/>
       <x:c r="D19" s="358" t="s"/>
       <x:c r="E19" s="248" t="s">
-        <x:v>60</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="F19" s="295" t="s"/>
       <x:c r="G19" s="357" t="s"/>
@@ -5055,7 +5065,7 @@
       <x:c r="I19" s="392" t="s"/>
       <x:c r="J19" s="357" t="s"/>
       <x:c r="K19" s="399" t="s">
-        <x:v>61</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="L19" s="400" t="s"/>
       <x:c r="M19" s="357" t="s"/>
@@ -5063,7 +5073,7 @@
     <x:row r="20" spans="1:15" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A20" s="357" t="s"/>
       <x:c r="B20" s="365" t="s">
-        <x:v>62</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="C20" s="401" t="s"/>
       <x:c r="D20" s="358" t="s"/>
@@ -5074,7 +5084,7 @@
       <x:c r="I20" s="357" t="s"/>
       <x:c r="J20" s="357" t="s"/>
       <x:c r="K20" s="402" t="s">
-        <x:v>63</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="L20" s="403">
         <x:f>'Rental Model'!C9</x:f>
@@ -5084,12 +5094,12 @@
     <x:row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <x:c r="A21" s="357" t="s"/>
       <x:c r="B21" s="243" t="s">
-        <x:v>64</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="C21" s="394" t="s"/>
       <x:c r="D21" s="358" t="s"/>
       <x:c r="E21" s="404" t="s">
-        <x:v>65</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="F21" s="405" t="s"/>
       <x:c r="G21" s="405" t="s"/>
@@ -5097,7 +5107,7 @@
       <x:c r="I21" s="406" t="s"/>
       <x:c r="J21" s="357" t="s"/>
       <x:c r="K21" s="407" t="s">
-        <x:v>66</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="L21" s="403">
         <x:f>'Rental Model'!F11</x:f>
@@ -5107,7 +5117,7 @@
     <x:row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <x:c r="A22" s="357" t="s"/>
       <x:c r="B22" s="244" t="s">
-        <x:v>67</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="C22" s="281" t="s"/>
       <x:c r="D22" s="358" t="s"/>
@@ -5118,7 +5128,7 @@
       <x:c r="I22" s="410" t="s"/>
       <x:c r="J22" s="357" t="s"/>
       <x:c r="K22" s="407" t="s">
-        <x:v>68</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="L22" s="411" t="e">
         <x:f>'Rental Model'!H3</x:f>
@@ -5128,7 +5138,7 @@
     <x:row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <x:c r="A23" s="357" t="s"/>
       <x:c r="B23" s="244" t="s">
-        <x:v>69</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="C23" s="281" t="s"/>
       <x:c r="D23" s="358" t="s"/>
@@ -5139,7 +5149,7 @@
       <x:c r="I23" s="410" t="s"/>
       <x:c r="J23" s="357" t="s"/>
       <x:c r="K23" s="407" t="s">
-        <x:v>70</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="L23" s="412" t="e">
         <x:f>'Rental Model'!C4</x:f>
@@ -5149,7 +5159,7 @@
     <x:row r="24" spans="1:15" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A24" s="357" t="s"/>
       <x:c r="B24" s="244" t="s">
-        <x:v>71</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="C24" s="284" t="s"/>
       <x:c r="D24" s="358" t="s"/>
@@ -5160,7 +5170,7 @@
       <x:c r="I24" s="410" t="s"/>
       <x:c r="J24" s="357" t="s"/>
       <x:c r="K24" s="413" t="s">
-        <x:v>72</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="L24" s="414" t="e">
         <x:f>'Rental Model'!H7</x:f>
@@ -5170,7 +5180,7 @@
     <x:row r="25" spans="1:15" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A25" s="357" t="s"/>
       <x:c r="B25" s="359" t="s">
-        <x:v>73</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="C25" s="415" t="n">
         <x:v>0.05</x:v>
@@ -5189,7 +5199,7 @@
     <x:row r="26" spans="1:15" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A26" s="357" t="s"/>
       <x:c r="B26" s="387" t="s">
-        <x:v>74</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="C26" s="416" t="n">
         <x:v>0.3</x:v>
@@ -5202,7 +5212,7 @@
       <x:c r="I26" s="410" t="s"/>
       <x:c r="J26" s="357" t="s"/>
       <x:c r="K26" s="417" t="s">
-        <x:v>75</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="L26" s="418" t="e">
         <x:f>Tables!H29-Tables!H22</x:f>
@@ -5227,7 +5237,7 @@
     <x:row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <x:c r="A28" s="357" t="s"/>
       <x:c r="B28" s="404" t="s">
-        <x:v>76</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="C28" s="420" t="s"/>
       <x:c r="D28" s="358" t="s"/>
@@ -5243,7 +5253,7 @@
     <x:row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <x:c r="A29" s="357" t="s"/>
       <x:c r="B29" s="244" t="s">
-        <x:v>77</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="C29" s="281" t="s"/>
       <x:c r="D29" s="358" t="s"/>
@@ -5260,7 +5270,7 @@
     <x:row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <x:c r="A30" s="357" t="s"/>
       <x:c r="B30" s="243" t="s">
-        <x:v>78</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="C30" s="287" t="s"/>
       <x:c r="D30" s="358" t="s"/>
@@ -5277,7 +5287,7 @@
     <x:row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <x:c r="A31" s="357" t="s"/>
       <x:c r="B31" s="244" t="s">
-        <x:v>79</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="C31" s="281" t="s"/>
       <x:c r="D31" s="358" t="s"/>
@@ -5294,7 +5304,7 @@
     <x:row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <x:c r="A32" s="357" t="s"/>
       <x:c r="B32" s="244" t="s">
-        <x:v>80</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="C32" s="288" t="s"/>
       <x:c r="D32" s="358" t="s"/>
@@ -5311,7 +5321,7 @@
     <x:row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <x:c r="A33" s="357" t="s"/>
       <x:c r="B33" s="244" t="s">
-        <x:v>81</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="C33" s="281" t="s"/>
       <x:c r="D33" s="358" t="s"/>
@@ -5328,7 +5338,7 @@
     <x:row r="34" spans="1:15" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A34" s="357" t="s"/>
       <x:c r="B34" s="422" t="s">
-        <x:v>82</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="C34" s="423" t="s"/>
       <x:c r="D34" s="357" t="s"/>
@@ -5524,7 +5534,7 @@
       <x:c r="F2" s="439" t="s"/>
       <x:c r="G2" s="430" t="s"/>
       <x:c r="H2" s="440" t="s">
-        <x:v>83</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="I2" s="430" t="s"/>
     </x:row>
@@ -5552,52 +5562,52 @@
     <x:row r="4" spans="1:12" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A4" s="430" t="s"/>
       <x:c r="B4" s="447" t="s">
-        <x:v>84</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="C4" s="448" t="s"/>
       <x:c r="D4" s="433" t="s"/>
       <x:c r="E4" s="447" t="s">
-        <x:v>85</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="F4" s="448" t="s"/>
       <x:c r="G4" s="449" t="s"/>
       <x:c r="H4" s="450" t="s">
-        <x:v>86</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="I4" s="430" t="s"/>
     </x:row>
     <x:row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <x:c r="A5" s="430" t="s"/>
       <x:c r="B5" s="451" t="s">
-        <x:v>87</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="C5" s="452" t="e">
         <x:f>SUM(Tables!K6:K8)</x:f>
       </x:c>
       <x:c r="D5" s="433" t="s"/>
       <x:c r="E5" s="451" t="s">
-        <x:v>88</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="F5" s="453">
         <x:f>Tables!O6</x:f>
       </x:c>
       <x:c r="G5" s="449" t="s"/>
       <x:c r="H5" s="454" t="s">
-        <x:v>89</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="I5" s="430" t="s"/>
     </x:row>
     <x:row r="6" spans="1:12" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A6" s="430" t="s"/>
       <x:c r="B6" s="431" t="s">
-        <x:v>90</x:v>
+        <x:v>92</x:v>
       </x:c>
       <x:c r="C6" s="455">
         <x:f>SUM(Tables!K9:K16)</x:f>
       </x:c>
       <x:c r="D6" s="433" t="s"/>
       <x:c r="E6" s="431" t="s">
-        <x:v>91</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="F6" s="434">
         <x:f>Tables!O7</x:f>
@@ -5611,35 +5621,35 @@
     <x:row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <x:c r="A7" s="430" t="s"/>
       <x:c r="B7" s="431" t="s">
-        <x:v>49</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="C7" s="455">
         <x:f>SUM(Tables!K18:K22)</x:f>
       </x:c>
       <x:c r="D7" s="433" t="s"/>
       <x:c r="E7" s="431" t="s">
-        <x:v>92</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="F7" s="434">
         <x:f>Tables!O8</x:f>
       </x:c>
       <x:c r="G7" s="449" t="s"/>
       <x:c r="H7" s="454" t="s">
-        <x:v>93</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="I7" s="430" t="s"/>
     </x:row>
     <x:row r="8" spans="1:12" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A8" s="430" t="s"/>
       <x:c r="B8" s="431" t="s">
-        <x:v>94</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="C8" s="455" t="e">
         <x:f>SUM(Tables!K24:K26)</x:f>
       </x:c>
       <x:c r="D8" s="433" t="s"/>
       <x:c r="E8" s="431" t="s">
-        <x:v>94</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="F8" s="434" t="e">
         <x:f>SUM(Tables!O9:O11)</x:f>
@@ -5653,7 +5663,7 @@
     <x:row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <x:c r="A9" s="430" t="s"/>
       <x:c r="B9" s="431" t="s">
-        <x:v>95</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="C9" s="455">
         <x:f>SUM(Tables!K28:K29)</x:f>
@@ -5669,7 +5679,7 @@
     <x:row r="10" spans="1:12" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A10" s="430" t="s"/>
       <x:c r="B10" s="431" t="s">
-        <x:v>96</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="C10" s="455">
         <x:f>SUM(Tables!K31:K33)</x:f>
@@ -5684,14 +5694,14 @@
     <x:row r="11" spans="1:12" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A11" s="430" t="s"/>
       <x:c r="B11" s="461" t="s">
-        <x:v>97</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="C11" s="462" t="e">
         <x:f>SUM(C5:C10)</x:f>
       </x:c>
       <x:c r="D11" s="433" t="s"/>
       <x:c r="E11" s="463" t="s">
-        <x:v>98</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F11" s="464" t="e">
         <x:f>F5-SUM(F6:F10)-C11</x:f>
@@ -5746,7 +5756,7 @@
       <x:c r="F15" s="439" t="s"/>
       <x:c r="G15" s="430" t="s"/>
       <x:c r="H15" s="468" t="s">
-        <x:v>83</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="I15" s="430" t="s"/>
     </x:row>
@@ -5774,52 +5784,52 @@
     <x:row r="17" spans="1:12" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A17" s="430" t="s"/>
       <x:c r="B17" s="470" t="s">
-        <x:v>84</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="C17" s="471" t="s"/>
       <x:c r="D17" s="433" t="s"/>
       <x:c r="E17" s="470" t="s">
-        <x:v>85</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="F17" s="471" t="s"/>
       <x:c r="G17" s="435" t="s"/>
       <x:c r="H17" s="472" t="s">
-        <x:v>99</x:v>
+        <x:v>101</x:v>
       </x:c>
       <x:c r="I17" s="430" t="s"/>
     </x:row>
     <x:row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <x:c r="A18" s="430" t="s"/>
       <x:c r="B18" s="451" t="s">
-        <x:v>100</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="C18" s="473" t="e">
         <x:f>SUM(Tables!K6:K8)</x:f>
       </x:c>
       <x:c r="D18" s="433" t="s"/>
       <x:c r="E18" s="451" t="s">
-        <x:v>88</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="F18" s="453">
         <x:f>Tables!O6</x:f>
       </x:c>
       <x:c r="G18" s="435" t="s"/>
       <x:c r="H18" s="454" t="s">
-        <x:v>101</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="I18" s="430" t="s"/>
     </x:row>
     <x:row r="19" spans="1:12" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A19" s="430" t="s"/>
       <x:c r="B19" s="431" t="s">
-        <x:v>102</x:v>
+        <x:v>104</x:v>
       </x:c>
       <x:c r="C19" s="432">
         <x:f>SUM(Tables!K9:K16)</x:f>
       </x:c>
       <x:c r="D19" s="433" t="s"/>
       <x:c r="E19" s="431" t="s">
-        <x:v>91</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="F19" s="434">
         <x:f>Tables!O7</x:f>
@@ -5833,35 +5843,35 @@
     <x:row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <x:c r="A20" s="430" t="s"/>
       <x:c r="B20" s="431" t="s">
-        <x:v>49</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="C20" s="432">
         <x:f>SUM(Tables!K18:K22)</x:f>
       </x:c>
       <x:c r="D20" s="433" t="s"/>
       <x:c r="E20" s="431" t="s">
-        <x:v>92</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="F20" s="434">
         <x:f>Tables!O8</x:f>
       </x:c>
       <x:c r="G20" s="435" t="s"/>
       <x:c r="H20" s="454" t="s">
-        <x:v>103</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="I20" s="430" t="s"/>
     </x:row>
     <x:row r="21" spans="1:12" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A21" s="430" t="s"/>
       <x:c r="B21" s="431" t="s">
-        <x:v>94</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="C21" s="474" t="e">
         <x:f>SUM(Tables!K24:K26)</x:f>
       </x:c>
       <x:c r="D21" s="433" t="s"/>
       <x:c r="E21" s="431" t="s">
-        <x:v>94</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="F21" s="434" t="e">
         <x:f>SUM(Tables!O9:O11)</x:f>
@@ -5875,7 +5885,7 @@
     <x:row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <x:c r="A22" s="430" t="s"/>
       <x:c r="B22" s="431" t="s">
-        <x:v>95</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="C22" s="432">
         <x:f>SUM(Tables!K28:K29)</x:f>
@@ -5885,14 +5895,14 @@
       <x:c r="F22" s="434" t="s"/>
       <x:c r="G22" s="435" t="s"/>
       <x:c r="H22" s="454" t="s">
-        <x:v>89</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="I22" s="430" t="s"/>
     </x:row>
     <x:row r="23" spans="1:12" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A23" s="430" t="s"/>
       <x:c r="B23" s="431" t="s">
-        <x:v>96</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="C23" s="432">
         <x:f>SUM(Tables!K31:K33)</x:f>
@@ -5909,7 +5919,7 @@
     <x:row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <x:c r="A24" s="430" t="s"/>
       <x:c r="B24" s="431" t="s">
-        <x:v>104</x:v>
+        <x:v>106</x:v>
       </x:c>
       <x:c r="C24" s="432" t="e">
         <x:f>SUM(Tables!O19:O21)</x:f>
@@ -5919,14 +5929,14 @@
       <x:c r="F24" s="434" t="s"/>
       <x:c r="G24" s="449" t="s"/>
       <x:c r="H24" s="454" t="s">
-        <x:v>93</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="I24" s="430" t="s"/>
     </x:row>
     <x:row r="25" spans="1:12" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A25" s="430" t="s"/>
       <x:c r="B25" s="431" t="s">
-        <x:v>105</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="C25" s="432">
         <x:f>Tables!O22</x:f>
@@ -5943,14 +5953,14 @@
     <x:row r="26" spans="1:12" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A26" s="430" t="s"/>
       <x:c r="B26" s="461" t="s">
-        <x:v>97</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="C26" s="478" t="e">
         <x:f>SUM(C18:C25)</x:f>
       </x:c>
       <x:c r="D26" s="433" t="s"/>
       <x:c r="E26" s="461" t="s">
-        <x:v>98</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F26" s="479" t="e">
         <x:f>F18-SUM(F19:F25)-C26</x:f>
@@ -6029,31 +6039,31 @@
     <x:row r="32" spans="1:12" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A32" s="430" t="s"/>
       <x:c r="B32" s="484" t="s">
-        <x:v>84</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="C32" s="485" t="s"/>
       <x:c r="D32" s="433" t="s"/>
       <x:c r="E32" s="484" t="s">
-        <x:v>106</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="F32" s="485" t="s"/>
       <x:c r="G32" s="449" t="s"/>
       <x:c r="H32" s="486" t="s">
-        <x:v>107</x:v>
+        <x:v>109</x:v>
       </x:c>
       <x:c r="I32" s="430" t="s"/>
     </x:row>
     <x:row r="33" spans="1:12" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A33" s="430" t="s"/>
       <x:c r="B33" s="487" t="s">
-        <x:v>108</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="C33" s="488" t="e">
         <x:f>SUM(Tables!K6:K22)</x:f>
       </x:c>
       <x:c r="D33" s="433" t="s"/>
       <x:c r="E33" s="487" t="s">
-        <x:v>88</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="F33" s="489" t="e">
         <x:f>Tables!D23</x:f>
@@ -6078,52 +6088,52 @@
     <x:row r="35" spans="1:12" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A35" s="430" t="s"/>
       <x:c r="B35" s="484" t="s">
-        <x:v>84</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="C35" s="485" t="s"/>
       <x:c r="D35" s="433" t="s"/>
       <x:c r="E35" s="484" t="s">
-        <x:v>85</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="F35" s="485" t="s"/>
       <x:c r="G35" s="449" t="s"/>
       <x:c r="H35" s="486" t="s">
-        <x:v>109</x:v>
+        <x:v>111</x:v>
       </x:c>
       <x:c r="I35" s="430" t="s"/>
     </x:row>
     <x:row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <x:c r="A36" s="430" t="s"/>
       <x:c r="B36" s="451" t="s">
-        <x:v>100</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="C36" s="473" t="e">
         <x:f>F33</x:f>
       </x:c>
       <x:c r="D36" s="433" t="s"/>
       <x:c r="E36" s="451" t="s">
-        <x:v>88</x:v>
+        <x:v>90</x:v>
       </x:c>
       <x:c r="F36" s="453">
         <x:f>Tables!O6</x:f>
       </x:c>
       <x:c r="G36" s="449" t="s"/>
       <x:c r="H36" s="454" t="s">
-        <x:v>89</x:v>
+        <x:v>91</x:v>
       </x:c>
       <x:c r="I36" s="430" t="s"/>
     </x:row>
     <x:row r="37" spans="1:12" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A37" s="430" t="s"/>
       <x:c r="B37" s="431" t="s">
-        <x:v>94</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="C37" s="432" t="e">
         <x:f>SUM(Tables!K24:K26)</x:f>
       </x:c>
       <x:c r="D37" s="433" t="s"/>
       <x:c r="E37" s="431" t="s">
-        <x:v>91</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="F37" s="434">
         <x:f>Tables!O7</x:f>
@@ -6137,35 +6147,35 @@
     <x:row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <x:c r="A38" s="430" t="s"/>
       <x:c r="B38" s="431" t="s">
-        <x:v>95</x:v>
+        <x:v>97</x:v>
       </x:c>
       <x:c r="C38" s="432">
         <x:f>SUM(Tables!K28:K29)</x:f>
       </x:c>
       <x:c r="D38" s="433" t="s"/>
       <x:c r="E38" s="431" t="s">
-        <x:v>92</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="F38" s="434">
         <x:f>Tables!O8</x:f>
       </x:c>
       <x:c r="G38" s="449" t="s"/>
       <x:c r="H38" s="454" t="s">
-        <x:v>93</x:v>
+        <x:v>95</x:v>
       </x:c>
       <x:c r="I38" s="430" t="s"/>
     </x:row>
     <x:row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <x:c r="A39" s="430" t="s"/>
       <x:c r="B39" s="431" t="s">
-        <x:v>96</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="C39" s="432">
         <x:f>SUM(Tables!K31:K33)</x:f>
       </x:c>
       <x:c r="D39" s="433" t="s"/>
       <x:c r="E39" s="431" t="s">
-        <x:v>94</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="F39" s="434" t="e">
         <x:f>SUM(Tables!O9:O11)</x:f>
@@ -6179,14 +6189,14 @@
     <x:row r="40" spans="1:12" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A40" s="430" t="s"/>
       <x:c r="B40" s="461" t="s">
-        <x:v>97</x:v>
+        <x:v>99</x:v>
       </x:c>
       <x:c r="C40" s="478" t="e">
         <x:f>SUM(C36:C39)</x:f>
       </x:c>
       <x:c r="D40" s="433" t="s"/>
       <x:c r="E40" s="461" t="s">
-        <x:v>98</x:v>
+        <x:v>100</x:v>
       </x:c>
       <x:c r="F40" s="479" t="e">
         <x:f>F36-SUM(F38:F39)-C40</x:f>
@@ -6276,25 +6286,25 @@
       <x:c r="I1" s="430" t="s"/>
       <x:c r="J1" s="357" t="s"/>
       <x:c r="K1" s="357" t="s">
-        <x:v>110</x:v>
+        <x:v>112</x:v>
       </x:c>
       <x:c r="L1" s="357" t="s">
-        <x:v>111</x:v>
+        <x:v>113</x:v>
       </x:c>
       <x:c r="M1" s="362" t="s">
-        <x:v>112</x:v>
+        <x:v>114</x:v>
       </x:c>
       <x:c r="N1" s="362" t="s">
-        <x:v>113</x:v>
+        <x:v>115</x:v>
       </x:c>
       <x:c r="O1" s="492" t="s">
-        <x:v>93</x:v>
+        <x:v>95</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <x:c r="A2" s="430" t="s"/>
       <x:c r="B2" s="493" t="s">
-        <x:v>114</x:v>
+        <x:v>116</x:v>
       </x:c>
       <x:c r="C2" s="438">
         <x:f>'Data Input'!C3</x:f>
@@ -6304,7 +6314,7 @@
       <x:c r="F2" s="439" t="s"/>
       <x:c r="G2" s="430" t="s"/>
       <x:c r="H2" s="494" t="s">
-        <x:v>68</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="I2" s="430" t="s"/>
       <x:c r="J2" s="357" t="s"/>
@@ -6324,14 +6334,14 @@
     <x:row r="3" spans="1:15" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A3" s="430" t="s"/>
       <x:c r="B3" s="495" t="s">
-        <x:v>115</x:v>
+        <x:v>117</x:v>
       </x:c>
       <x:c r="C3" s="436">
         <x:f>'Data Input'!C32</x:f>
       </x:c>
       <x:c r="D3" s="436" t="s"/>
       <x:c r="E3" s="430" t="s">
-        <x:v>116</x:v>
+        <x:v>118</x:v>
       </x:c>
       <x:c r="F3" s="496" t="n">
         <x:v>0.16</x:v>
@@ -6361,21 +6371,21 @@
     <x:row r="4" spans="1:15" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A4" s="430" t="s"/>
       <x:c r="B4" s="497" t="s">
-        <x:v>117</x:v>
+        <x:v>119</x:v>
       </x:c>
       <x:c r="C4" s="442" t="e">
         <x:f>IF('Data Input'!C34="",MATCH(1,INDEX(--(O2:O97&gt;F4),0),0),'Data Input'!C34)</x:f>
       </x:c>
       <x:c r="D4" s="442" t="s"/>
       <x:c r="E4" s="443" t="s">
-        <x:v>118</x:v>
+        <x:v>120</x:v>
       </x:c>
       <x:c r="F4" s="498" t="n">
         <x:v>0.18</x:v>
       </x:c>
       <x:c r="G4" s="430" t="s"/>
       <x:c r="H4" s="499" t="s">
-        <x:v>119</x:v>
+        <x:v>121</x:v>
       </x:c>
       <x:c r="I4" s="430" t="s"/>
       <x:c r="J4" s="357" t="s"/>
@@ -6398,12 +6408,12 @@
     <x:row r="5" spans="1:15" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A5" s="430" t="s"/>
       <x:c r="B5" s="500" t="s">
-        <x:v>120</x:v>
+        <x:v>122</x:v>
       </x:c>
       <x:c r="C5" s="501" t="s"/>
       <x:c r="D5" s="430" t="s"/>
       <x:c r="E5" s="502" t="s">
-        <x:v>121</x:v>
+        <x:v>123</x:v>
       </x:c>
       <x:c r="F5" s="503" t="s"/>
       <x:c r="G5" s="430" t="s"/>
@@ -6431,21 +6441,21 @@
     <x:row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <x:c r="A6" s="430" t="s"/>
       <x:c r="B6" s="505" t="s">
-        <x:v>122</x:v>
+        <x:v>124</x:v>
       </x:c>
       <x:c r="C6" s="435">
         <x:f>'Data Input'!C29</x:f>
       </x:c>
       <x:c r="D6" s="449" t="s"/>
       <x:c r="E6" s="431" t="s">
-        <x:v>113</x:v>
+        <x:v>115</x:v>
       </x:c>
       <x:c r="F6" s="435">
         <x:f>'Data Input'!C33</x:f>
       </x:c>
       <x:c r="G6" s="430" t="s"/>
       <x:c r="H6" s="506" t="s">
-        <x:v>72</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="I6" s="430" t="s"/>
       <x:c r="J6" s="357" t="s"/>
@@ -6468,14 +6478,14 @@
     <x:row r="7" spans="1:15" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A7" s="430" t="s"/>
       <x:c r="B7" s="507" t="s">
-        <x:v>123</x:v>
+        <x:v>125</x:v>
       </x:c>
       <x:c r="C7" s="435">
         <x:f>'Data Input'!C31</x:f>
       </x:c>
       <x:c r="D7" s="449" t="s"/>
       <x:c r="E7" s="431" t="s">
-        <x:v>124</x:v>
+        <x:v>126</x:v>
       </x:c>
       <x:c r="F7" s="435">
         <x:f>F6*0.1</x:f>
@@ -6505,21 +6515,21 @@
     <x:row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <x:c r="A8" s="430" t="s"/>
       <x:c r="B8" s="431" t="s">
-        <x:v>58</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="C8" s="435">
         <x:f>'Data Input'!C18</x:f>
       </x:c>
       <x:c r="D8" s="449" t="s"/>
       <x:c r="E8" s="431" t="s">
-        <x:v>125</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="F8" s="435" t="n">
         <x:v>85</x:v>
       </x:c>
       <x:c r="G8" s="430" t="s"/>
       <x:c r="H8" s="494" t="s">
-        <x:v>126</x:v>
+        <x:v>128</x:v>
       </x:c>
       <x:c r="I8" s="430" t="s"/>
       <x:c r="J8" s="357" t="s"/>
@@ -6542,14 +6552,14 @@
     <x:row r="9" spans="1:15" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A9" s="430" t="s"/>
       <x:c r="B9" s="431" t="s">
-        <x:v>127</x:v>
+        <x:v>129</x:v>
       </x:c>
       <x:c r="C9" s="435">
         <x:f>SUM(C6:C8)</x:f>
       </x:c>
       <x:c r="D9" s="449" t="s"/>
       <x:c r="E9" s="431" t="s">
-        <x:v>128</x:v>
+        <x:v>130</x:v>
       </x:c>
       <x:c r="F9" s="435">
         <x:f>50+((C3-1)*25)</x:f>
@@ -6579,21 +6589,21 @@
     <x:row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <x:c r="A10" s="430" t="s"/>
       <x:c r="B10" s="431" t="s">
-        <x:v>116</x:v>
+        <x:v>118</x:v>
       </x:c>
       <x:c r="C10" s="435">
         <x:f>-SUM(M2:M61)</x:f>
       </x:c>
       <x:c r="D10" s="430" t="s"/>
       <x:c r="E10" s="431" t="s">
-        <x:v>129</x:v>
+        <x:v>131</x:v>
       </x:c>
       <x:c r="F10" s="435">
         <x:f>75*C3</x:f>
       </x:c>
       <x:c r="G10" s="430" t="s"/>
       <x:c r="H10" s="494" t="s">
-        <x:v>130</x:v>
+        <x:v>132</x:v>
       </x:c>
       <x:c r="I10" s="430" t="s"/>
       <x:c r="J10" s="357" t="s"/>
@@ -6616,14 +6626,14 @@
     <x:row r="11" spans="1:15" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A11" s="430" t="s"/>
       <x:c r="B11" s="510" t="s">
-        <x:v>108</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="C11" s="479">
         <x:f>C9+C10</x:f>
       </x:c>
       <x:c r="D11" s="449" t="s"/>
       <x:c r="E11" s="510" t="s">
-        <x:v>131</x:v>
+        <x:v>133</x:v>
       </x:c>
       <x:c r="F11" s="479">
         <x:f>F6-SUM(F7:F10)</x:f>
@@ -8277,10 +8287,10 @@
   <x:sheetData>
     <x:row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <x:c r="A1" s="520" t="s">
-        <x:v>132</x:v>
+        <x:v>134</x:v>
       </x:c>
       <x:c r="C1" s="521" t="s">
-        <x:v>133</x:v>
+        <x:v>135</x:v>
       </x:c>
       <x:c r="D1" s="522" t="s"/>
       <x:c r="E1" s="523" t="s"/>
@@ -8297,7 +8307,7 @@
       <x:c r="M1" s="345" t="s"/>
       <x:c r="N1" s="345" t="s"/>
       <x:c r="O1" s="136" t="s">
-        <x:v>134</x:v>
+        <x:v>136</x:v>
       </x:c>
       <x:c r="P1" s="165">
         <x:f>'Data Input'!C24</x:f>
@@ -8308,14 +8318,14 @@
     <x:row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <x:c r="A2" s="527" t="s"/>
       <x:c r="C2" s="9" t="s">
-        <x:v>100</x:v>
+        <x:v>102</x:v>
       </x:c>
       <x:c r="D2" s="528" t="s">
-        <x:v>135</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="E2" s="528" t="s"/>
       <x:c r="F2" s="529" t="s">
-        <x:v>136</x:v>
+        <x:v>138</x:v>
       </x:c>
       <x:c r="G2" s="529" t="s"/>
       <x:c r="H2" s="10" t="s"/>
@@ -8331,7 +8341,7 @@
       </x:c>
       <x:c r="N2" s="533" t="s"/>
       <x:c r="O2" s="534" t="s">
-        <x:v>137</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="P2" s="535">
         <x:f>'Data Input'!C26</x:f>
@@ -8341,7 +8351,7 @@
     </x:row>
     <x:row r="3" spans="1:21" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A3" s="536" t="s">
-        <x:v>138</x:v>
+        <x:v>140</x:v>
       </x:c>
       <x:c r="C3" s="11" t="e">
         <x:f>Tables!K6</x:f>
@@ -8356,20 +8366,20 @@
       <x:c r="G3" s="537" t="s"/>
       <x:c r="H3" s="10" t="s"/>
       <x:c r="J3" s="51" t="s">
-        <x:v>139</x:v>
+        <x:v>141</x:v>
       </x:c>
       <x:c r="K3" s="141">
         <x:f>'Data Input'!C10</x:f>
       </x:c>
       <x:c r="L3" s="142" t="s"/>
       <x:c r="M3" s="143" t="s">
-        <x:v>42</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="N3" s="60">
         <x:f>'Data Input'!C12</x:f>
       </x:c>
       <x:c r="O3" s="143" t="s">
-        <x:v>140</x:v>
+        <x:v>142</x:v>
       </x:c>
       <x:c r="P3" s="169" t="n">
         <x:v>0</x:v>
@@ -8379,7 +8389,7 @@
     </x:row>
     <x:row r="4" spans="1:21" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A4" s="538" t="s">
-        <x:v>141</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="C4" s="12" t="s"/>
       <x:c r="D4" s="355" t="s"/>
@@ -8391,45 +8401,45 @@
     </x:row>
     <x:row r="5" spans="1:21" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A5" s="538" t="s">
-        <x:v>142</x:v>
+        <x:v>144</x:v>
       </x:c>
       <x:c r="C5" s="14" t="s">
-        <x:v>143</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="D5" s="539" t="s">
-        <x:v>144</x:v>
+        <x:v>146</x:v>
       </x:c>
       <x:c r="E5" s="539" t="s">
-        <x:v>145</x:v>
+        <x:v>147</x:v>
       </x:c>
       <x:c r="F5" s="539" t="s">
-        <x:v>146</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="G5" s="539" t="s">
-        <x:v>147</x:v>
+        <x:v>149</x:v>
       </x:c>
       <x:c r="H5" s="16" t="s">
-        <x:v>148</x:v>
+        <x:v>150</x:v>
       </x:c>
       <x:c r="J5" s="540" t="s">
-        <x:v>149</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="K5" s="541" t="s"/>
       <x:c r="L5" s="542" t="s">
-        <x:v>150</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="N5" s="540" t="s">
-        <x:v>151</x:v>
+        <x:v>153</x:v>
       </x:c>
       <x:c r="O5" s="541" t="s"/>
       <x:c r="Q5" s="360" t="s">
-        <x:v>152</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="R5" s="361" t="s"/>
     </x:row>
     <x:row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <x:c r="A6" s="538" t="s">
-        <x:v>153</x:v>
+        <x:v>155</x:v>
       </x:c>
       <x:c r="C6" s="17" t="n">
         <x:v>35001</x:v>
@@ -8450,7 +8460,7 @@
         <x:f>((D6-C6)*F6)+344</x:f>
       </x:c>
       <x:c r="J6" s="127" t="s">
-        <x:v>87</x:v>
+        <x:v>89</x:v>
       </x:c>
       <x:c r="K6" s="145" t="e">
         <x:f>(O6-SUM(K7:K16,K18:K22,K25:K26,K28:K29,K31:K33,O7:O11)-(SUM(K7:K16,K18:K22,K25:K26,K28:K29,K31:K33)*P2))/((P2*1.0058)+1.0058)</x:f>
@@ -8459,7 +8469,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="N6" s="127" t="s">
-        <x:v>154</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="O6" s="145">
         <x:f>'Data Input'!C22</x:f>
@@ -8473,7 +8483,7 @@
     </x:row>
     <x:row r="7" spans="1:21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="A7" s="538" t="s">
-        <x:v>155</x:v>
+        <x:v>157</x:v>
       </x:c>
       <x:c r="C7" s="17" t="n">
         <x:v>50001</x:v>
@@ -8494,7 +8504,7 @@
         <x:f>((D7-C7)*F7)+H6</x:f>
       </x:c>
       <x:c r="J7" s="127" t="s">
-        <x:v>156</x:v>
+        <x:v>158</x:v>
       </x:c>
       <x:c r="K7" s="145">
         <x:f>'Data Input'!I3*(1+(L7*'Data Input'!C24))</x:f>
@@ -8503,13 +8513,13 @@
         <x:f>0.09/12</x:f>
       </x:c>
       <x:c r="N7" s="127" t="s">
-        <x:v>91</x:v>
+        <x:v>93</x:v>
       </x:c>
       <x:c r="O7" s="145" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="Q7" s="548" t="s">
-        <x:v>157</x:v>
+        <x:v>159</x:v>
       </x:c>
       <x:c r="R7" s="549" t="e">
         <x:f>'Flip Sheets'!F11</x:f>
@@ -8517,7 +8527,7 @@
     </x:row>
     <x:row r="8" spans="1:21" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A8" s="550" t="s">
-        <x:v>158</x:v>
+        <x:v>160</x:v>
       </x:c>
       <x:c r="C8" s="17" t="n">
         <x:v>100001</x:v>
@@ -8538,7 +8548,7 @@
         <x:f>((D8-C8)*F8)+H7</x:f>
       </x:c>
       <x:c r="J8" s="551" t="s">
-        <x:v>159</x:v>
+        <x:v>161</x:v>
       </x:c>
       <x:c r="K8" s="145">
         <x:f>'Data Input'!I4*L8</x:f>
@@ -8547,13 +8557,13 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="N8" s="127" t="s">
-        <x:v>92</x:v>
+        <x:v>94</x:v>
       </x:c>
       <x:c r="O8" s="145">
         <x:f>O6*'Data Input'!C25</x:f>
       </x:c>
       <x:c r="Q8" s="548" t="s">
-        <x:v>160</x:v>
+        <x:v>162</x:v>
       </x:c>
       <x:c r="R8" s="552" t="e">
         <x:f>'Flip Sheets'!H8</x:f>
@@ -8580,7 +8590,7 @@
         <x:f>((D9-C9)*F9)+H8</x:f>
       </x:c>
       <x:c r="J9" s="127" t="s">
-        <x:v>161</x:v>
+        <x:v>163</x:v>
       </x:c>
       <x:c r="K9" s="145">
         <x:f>'Data Input'!I5*L9</x:f>
@@ -8589,13 +8599,13 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="N9" s="127" t="s">
-        <x:v>162</x:v>
+        <x:v>164</x:v>
       </x:c>
       <x:c r="O9" s="145" t="e">
         <x:f>(IF('Data Input'!C2="Residential",IF(AND(O6&gt;0,O6&lt;=500000),"1%",IF(O6&gt;500000,"1.425%","")),IF(AND(O6&gt;0,O6&lt;=500000),"1.425%",IF(O6&gt;500000,"2.625%","")))+0.4%)*O6</x:f>
       </x:c>
       <x:c r="Q9" s="553" t="s">
-        <x:v>163</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="R9" s="554" t="e">
         <x:f>R8/'Data Input'!C24*12</x:f>
@@ -8603,7 +8613,7 @@
     </x:row>
     <x:row r="10" spans="1:21" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A10" s="520" t="s">
-        <x:v>164</x:v>
+        <x:v>166</x:v>
       </x:c>
       <x:c r="C10" s="17" t="n">
         <x:v>1000001</x:v>
@@ -8624,7 +8634,7 @@
         <x:f>((D10-C10)*F10)+H9</x:f>
       </x:c>
       <x:c r="J10" s="127" t="s">
-        <x:v>165</x:v>
+        <x:v>167</x:v>
       </x:c>
       <x:c r="K10" s="145">
         <x:f>'Data Input'!I6*L10</x:f>
@@ -8633,7 +8643,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="N10" s="127" t="s">
-        <x:v>166</x:v>
+        <x:v>168</x:v>
       </x:c>
       <x:c r="O10" s="145" t="n">
         <x:v>1250</x:v>
@@ -8662,7 +8672,7 @@
         <x:f>((D11-C11)*F11)+H10</x:f>
       </x:c>
       <x:c r="J11" s="127" t="s">
-        <x:v>167</x:v>
+        <x:v>169</x:v>
       </x:c>
       <x:c r="K11" s="145">
         <x:f>('Data Input'!I7*(1+(P1*0.0075)))*L11</x:f>
@@ -8671,19 +8681,19 @@
         <x:v>0.35</x:v>
       </x:c>
       <x:c r="N11" s="127" t="s">
-        <x:v>168</x:v>
+        <x:v>170</x:v>
       </x:c>
       <x:c r="O11" s="145" t="n">
         <x:v>500</x:v>
       </x:c>
       <x:c r="Q11" s="555" t="s">
-        <x:v>169</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="R11" s="556" t="s"/>
     </x:row>
     <x:row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <x:c r="A12" s="536" t="s">
-        <x:v>170</x:v>
+        <x:v>172</x:v>
       </x:c>
       <x:c r="C12" s="17" t="n">
         <x:v>10000001</x:v>
@@ -8704,7 +8714,7 @@
         <x:f>((D12-C12)*F12)+H11</x:f>
       </x:c>
       <x:c r="J12" s="127" t="s">
-        <x:v>171</x:v>
+        <x:v>173</x:v>
       </x:c>
       <x:c r="K12" s="145">
         <x:f>'Data Input'!I8*L12</x:f>
@@ -8713,7 +8723,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="N12" s="540" t="s">
-        <x:v>172</x:v>
+        <x:v>174</x:v>
       </x:c>
       <x:c r="O12" s="557" t="s"/>
       <x:c r="Q12" s="558" t="s">
@@ -8725,7 +8735,7 @@
     </x:row>
     <x:row r="13" spans="1:21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="A13" s="538" t="s">
-        <x:v>173</x:v>
+        <x:v>175</x:v>
       </x:c>
       <x:c r="C13" s="17" t="n">
         <x:v>15000001</x:v>
@@ -8740,7 +8750,7 @@
       <x:c r="G13" s="512" t="s"/>
       <x:c r="H13" s="20" t="s"/>
       <x:c r="J13" s="127" t="s">
-        <x:v>174</x:v>
+        <x:v>176</x:v>
       </x:c>
       <x:c r="K13" s="145">
         <x:f>'Data Input'!I9*L13</x:f>
@@ -8749,13 +8759,13 @@
         <x:v>0.4</x:v>
       </x:c>
       <x:c r="N13" s="127" t="s">
-        <x:v>101</x:v>
+        <x:v>103</x:v>
       </x:c>
       <x:c r="O13" s="145">
         <x:f>O6*O17</x:f>
       </x:c>
       <x:c r="Q13" s="560" t="s">
-        <x:v>175</x:v>
+        <x:v>177</x:v>
       </x:c>
       <x:c r="R13" s="561" t="e">
         <x:f>'Flip Sheets'!F26</x:f>
@@ -8763,7 +8773,7 @@
     </x:row>
     <x:row r="14" spans="1:21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="A14" s="562" t="s">
-        <x:v>176</x:v>
+        <x:v>178</x:v>
       </x:c>
       <x:c r="C14" s="12" t="s"/>
       <x:c r="D14" s="355" t="s"/>
@@ -8772,7 +8782,7 @@
       <x:c r="G14" s="355" t="s"/>
       <x:c r="H14" s="10" t="s"/>
       <x:c r="J14" s="127" t="s">
-        <x:v>177</x:v>
+        <x:v>179</x:v>
       </x:c>
       <x:c r="K14" s="145">
         <x:f>'Data Input'!I10*L14</x:f>
@@ -8781,13 +8791,13 @@
         <x:v>0.15</x:v>
       </x:c>
       <x:c r="N14" s="127" t="s">
-        <x:v>178</x:v>
+        <x:v>180</x:v>
       </x:c>
       <x:c r="O14" s="128" t="n">
         <x:v>0.12</x:v>
       </x:c>
       <x:c r="Q14" s="560" t="s">
-        <x:v>179</x:v>
+        <x:v>181</x:v>
       </x:c>
       <x:c r="R14" s="563" t="e">
         <x:f>'Flip Sheets'!H25</x:f>
@@ -8795,24 +8805,24 @@
     </x:row>
     <x:row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <x:c r="A15" s="538" t="s">
-        <x:v>180</x:v>
+        <x:v>182</x:v>
       </x:c>
       <x:c r="C15" s="14" t="s">
-        <x:v>145</x:v>
+        <x:v>147</x:v>
       </x:c>
       <x:c r="D15" s="528" t="s">
-        <x:v>181</x:v>
+        <x:v>183</x:v>
       </x:c>
       <x:c r="E15" s="528" t="s"/>
       <x:c r="F15" s="355" t="s"/>
       <x:c r="G15" s="564" t="s">
-        <x:v>182</x:v>
+        <x:v>184</x:v>
       </x:c>
       <x:c r="H15" s="16" t="s">
-        <x:v>183</x:v>
+        <x:v>185</x:v>
       </x:c>
       <x:c r="J15" s="127" t="s">
-        <x:v>184</x:v>
+        <x:v>186</x:v>
       </x:c>
       <x:c r="K15" s="145">
         <x:f>'Data Input'!I11*L15</x:f>
@@ -8821,13 +8831,13 @@
         <x:f>IF('Data Input'!I11&lt;12500,100%,0%)</x:f>
       </x:c>
       <x:c r="N15" s="127" t="s">
-        <x:v>185</x:v>
+        <x:v>187</x:v>
       </x:c>
       <x:c r="O15" s="23" t="n">
         <x:v>2</x:v>
       </x:c>
       <x:c r="Q15" s="565" t="s">
-        <x:v>163</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="R15" s="566" t="e">
         <x:f>R14/'Data Input'!C24*12</x:f>
@@ -8835,7 +8845,7 @@
     </x:row>
     <x:row r="16" spans="1:21" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A16" s="538" t="s">
-        <x:v>186</x:v>
+        <x:v>188</x:v>
       </x:c>
       <x:c r="C16" s="21" t="e">
         <x:f>IF(C3&lt;C6,402,IF(C3&lt;=D6,(C3-C6)*E6,IF(C3&lt;=D7,(C3-C7)*E7+G6,IF(C3&lt;=D8,(C3-C8)*E8+G7,IF(C3&lt;=D9,(C3-C9)*E9+G8,IF(C3&lt;=D10,(C3-C10)*E10+G9,IF(C3&lt;=D11,(C3-C11)*E11+G10,IF(C3&lt;=D12,(C3-C12)*E12+G11,IF(C3&gt;=C13,(C3-C13)*E13+G12,"")))))))))</x:f>
@@ -8854,7 +8864,7 @@
         <x:f>D16+E16+G16</x:f>
       </x:c>
       <x:c r="J16" s="130" t="s">
-        <x:v>187</x:v>
+        <x:v>189</x:v>
       </x:c>
       <x:c r="K16" s="147">
         <x:f>IF('Data Input'!I14="",0,'Data Input'!I13*(1+(TODAY()+180-'Data Input'!I14)*L16))</x:f>
@@ -8863,7 +8873,7 @@
         <x:f>9%/365</x:f>
       </x:c>
       <x:c r="N16" s="127" t="s">
-        <x:v>188</x:v>
+        <x:v>190</x:v>
       </x:c>
       <x:c r="O16" s="23" t="n">
         <x:v>12</x:v>
@@ -8877,21 +8887,21 @@
     </x:row>
     <x:row r="17" spans="1:21" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A17" s="538" t="s">
-        <x:v>189</x:v>
+        <x:v>191</x:v>
       </x:c>
       <x:c r="J17" s="517" t="s">
-        <x:v>190</x:v>
+        <x:v>192</x:v>
       </x:c>
       <x:c r="K17" s="569" t="s"/>
       <x:c r="L17" s="570" t="s"/>
       <x:c r="N17" s="127" t="s">
-        <x:v>103</x:v>
+        <x:v>105</x:v>
       </x:c>
       <x:c r="O17" s="129" t="n">
         <x:v>0.6</x:v>
       </x:c>
       <x:c r="Q17" s="560" t="s">
-        <x:v>191</x:v>
+        <x:v>193</x:v>
       </x:c>
       <x:c r="R17" s="563" t="e">
         <x:f>R13/R16</x:f>
@@ -8899,33 +8909,33 @@
     </x:row>
     <x:row r="18" spans="1:21" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A18" s="550" t="s">
-        <x:v>192</x:v>
+        <x:v>194</x:v>
       </x:c>
       <x:c r="C18" s="521" t="s">
-        <x:v>162</x:v>
+        <x:v>164</x:v>
       </x:c>
       <x:c r="D18" s="571" t="s"/>
       <x:c r="F18" s="572" t="s"/>
       <x:c r="G18" s="573" t="s">
-        <x:v>193</x:v>
+        <x:v>195</x:v>
       </x:c>
       <x:c r="H18" s="574" t="n">
         <x:v>0.25</x:v>
       </x:c>
       <x:c r="I18" s="572" t="s"/>
       <x:c r="J18" s="127" t="s">
-        <x:v>194</x:v>
+        <x:v>196</x:v>
       </x:c>
       <x:c r="K18" s="145">
         <x:f>'Data Input'!C15</x:f>
       </x:c>
       <x:c r="L18" s="575" t="s"/>
       <x:c r="N18" s="517" t="s">
-        <x:v>195</x:v>
+        <x:v>197</x:v>
       </x:c>
       <x:c r="O18" s="576" t="s"/>
       <x:c r="Q18" s="577" t="s">
-        <x:v>196</x:v>
+        <x:v>198</x:v>
       </x:c>
       <x:c r="R18" s="578" t="e">
         <x:f>R17/'Data Input'!C24*12</x:f>
@@ -8934,7 +8944,7 @@
     <x:row r="19" spans="1:21" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A19" s="355" t="s"/>
       <x:c r="C19" s="579" t="s">
-        <x:v>197</x:v>
+        <x:v>199</x:v>
       </x:c>
       <x:c r="D19" s="56" t="str">
         <x:f>IF(OR(NOT(ISERROR(SEARCH(("A"),'Data Input'!C4))),NOT(ISERROR(SEARCH(("B"),'Data Input'!C4))),NOT(ISERROR(SEARCH(("C0"),'Data Input'!C4))),NOT(ISERROR(SEARCH(("21"),'Data Input'!C4))),NOT(ISERROR(SEARCH(("R"),'Data Input'!C4)))),"Residential","Not Residential")</x:f>
@@ -8948,7 +8958,7 @@
       </x:c>
       <x:c r="I19" s="514" t="s"/>
       <x:c r="J19" s="127" t="s">
-        <x:v>198</x:v>
+        <x:v>200</x:v>
       </x:c>
       <x:c r="K19" s="582">
         <x:f>IF(OR('Data Input'!C11="Yes",'Data Input'!C12&gt;0)*AND('Data Input'!F8&lt;&gt;"Yes",'Data Input'!F9&lt;&gt;"Yes",'Data Input'!F10&lt;&gt;"Yes",'Data Input'!C16&lt;&gt;""),'Data Input'!C16*L19-10000,'Data Input'!C16*L19)</x:f>
@@ -8957,7 +8967,7 @@
         <x:v>0.75</x:v>
       </x:c>
       <x:c r="N19" s="127" t="s">
-        <x:v>146</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="O19" s="179" t="e">
         <x:f>Tables!H16-Tables!C16</x:f>
@@ -8967,7 +8977,7 @@
     </x:row>
     <x:row r="20" spans="1:21" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A20" s="584" t="s">
-        <x:v>199</x:v>
+        <x:v>201</x:v>
       </x:c>
       <x:c r="F20" s="514" t="s"/>
       <x:c r="G20" s="585" t="s">
@@ -8978,27 +8988,27 @@
       </x:c>
       <x:c r="I20" s="514" t="s"/>
       <x:c r="J20" s="127" t="s">
-        <x:v>56</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="K20" s="145">
         <x:f>'Data Input'!C17</x:f>
       </x:c>
       <x:c r="L20" s="575" t="s"/>
       <x:c r="N20" s="127" t="s">
-        <x:v>200</x:v>
+        <x:v>202</x:v>
       </x:c>
       <x:c r="O20" s="145" t="e">
         <x:f>((IF('Data Input'!C2="Residential",IF(AND(O13&gt;0,O13&lt;=500000),"2.0%",IF(O13&gt;500000,"2.125%","")),IF(AND(O13&gt;0,O13&lt;=500000),"2.0%",IF(O13&gt;500000,"2.75%",""))))*O13)+(275)+1500</x:f>
       </x:c>
       <x:c r="Q20" s="587" t="s">
-        <x:v>201</x:v>
+        <x:v>203</x:v>
       </x:c>
       <x:c r="R20" s="588" t="s"/>
     </x:row>
     <x:row r="21" spans="1:21" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <x:c r="A21" s="589" t="s"/>
       <x:c r="C21" s="384" t="s">
-        <x:v>202</x:v>
+        <x:v>204</x:v>
       </x:c>
       <x:c r="D21" s="590" t="s"/>
       <x:c r="F21" s="514" t="s"/>
@@ -9010,20 +9020,20 @@
       </x:c>
       <x:c r="I21" s="514" t="s"/>
       <x:c r="J21" s="127" t="s">
-        <x:v>203</x:v>
+        <x:v>205</x:v>
       </x:c>
       <x:c r="K21" s="145">
         <x:f>'Data Input'!C12*5000</x:f>
       </x:c>
       <x:c r="L21" s="575" t="s"/>
       <x:c r="N21" s="127" t="s">
-        <x:v>204</x:v>
+        <x:v>206</x:v>
       </x:c>
       <x:c r="O21" s="145">
         <x:f>(O13*O15%)</x:f>
       </x:c>
       <x:c r="Q21" s="591" t="s">
-        <x:v>106</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="R21" s="592" t="e">
         <x:f>'Flip Sheets'!F33</x:f>
@@ -9031,37 +9041,37 @@
     </x:row>
     <x:row r="22" spans="1:21" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A22" s="513" t="s">
-        <x:v>45</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="C22" s="53" t="s">
-        <x:v>205</x:v>
+        <x:v>207</x:v>
       </x:c>
       <x:c r="D22" s="593" t="n">
         <x:v>0.15</x:v>
       </x:c>
       <x:c r="F22" s="514" t="s"/>
       <x:c r="G22" s="585" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="H22" s="594" t="e">
         <x:f>O6-SUM(O7:O11)-H20</x:f>
       </x:c>
       <x:c r="I22" s="514" t="s"/>
       <x:c r="J22" s="127" t="s">
-        <x:v>206</x:v>
+        <x:v>208</x:v>
       </x:c>
       <x:c r="K22" s="145">
         <x:f>'Data Input'!C18</x:f>
       </x:c>
       <x:c r="L22" s="575" t="s"/>
       <x:c r="N22" s="130" t="s">
-        <x:v>105</x:v>
+        <x:v>107</x:v>
       </x:c>
       <x:c r="O22" s="147">
         <x:f>(O13*O14/12*'Data Input'!C24)</x:f>
       </x:c>
       <x:c r="Q22" s="595" t="s">
-        <x:v>108</x:v>
+        <x:v>110</x:v>
       </x:c>
       <x:c r="R22" s="596" t="e">
         <x:f>'Flip Sheets'!C33</x:f>
@@ -9072,21 +9082,21 @@
         <x:v>15</x:v>
       </x:c>
       <x:c r="C23" s="54" t="s">
-        <x:v>106</x:v>
+        <x:v>108</x:v>
       </x:c>
       <x:c r="D23" s="96" t="e">
         <x:f>(Tables!O6-SUM(Tables!K24:K33,Tables!O7:O11)-(SUM(Tables!K24:K33)*Tables!D22))/((Tables!D22*1)+1)</x:f>
       </x:c>
       <x:c r="F23" s="514" t="s"/>
       <x:c r="G23" s="515" t="s">
-        <x:v>38</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="H23" s="516" t="e">
         <x:f>H22/H20</x:f>
       </x:c>
       <x:c r="I23" s="514" t="s"/>
       <x:c r="J23" s="517" t="s">
-        <x:v>94</x:v>
+        <x:v>96</x:v>
       </x:c>
       <x:c r="K23" s="518" t="s"/>
       <x:c r="L23" s="570" t="s"/>
@@ -9095,7 +9105,7 @@
       <x:c r="O23" s="598" t="s"/>
       <x:c r="P23" s="598" t="s"/>
       <x:c r="Q23" s="599" t="s">
-        <x:v>107</x:v>
+        <x:v>109</x:v>
       </x:c>
       <x:c r="R23" s="600" t="e">
         <x:f>R21-R22</x:f>
@@ -9108,7 +9118,7 @@
       <x:c r="H24" s="355" t="s"/>
       <x:c r="I24" s="572" t="s"/>
       <x:c r="J24" s="127" t="s">
-        <x:v>207</x:v>
+        <x:v>209</x:v>
       </x:c>
       <x:c r="K24" s="145" t="e">
         <x:f>Tables!C16</x:f>
@@ -9121,20 +9131,20 @@
     </x:row>
     <x:row r="25" spans="1:21" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A25" s="584" t="s">
-        <x:v>149</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="C25" s="521" t="s">
-        <x:v>208</x:v>
+        <x:v>210</x:v>
       </x:c>
       <x:c r="D25" s="590" t="s"/>
       <x:c r="F25" s="514" t="s"/>
       <x:c r="G25" s="573" t="s">
-        <x:v>209</x:v>
+        <x:v>211</x:v>
       </x:c>
       <x:c r="H25" s="574" t="s"/>
       <x:c r="I25" s="514" t="s"/>
       <x:c r="J25" s="127" t="s">
-        <x:v>210</x:v>
+        <x:v>212</x:v>
       </x:c>
       <x:c r="K25" s="145" t="n">
         <x:v>1200</x:v>
@@ -9148,7 +9158,7 @@
     <x:row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <x:c r="A26" s="513" t="s"/>
       <x:c r="C26" s="2" t="s">
-        <x:v>140</x:v>
+        <x:v>142</x:v>
       </x:c>
       <x:c r="D26" s="180" t="n">
         <x:v>0</x:v>
@@ -9162,7 +9172,7 @@
       </x:c>
       <x:c r="I26" s="514" t="s"/>
       <x:c r="J26" s="127" t="s">
-        <x:v>211</x:v>
+        <x:v>213</x:v>
       </x:c>
       <x:c r="K26" s="145" t="n">
         <x:v>1250</x:v>
@@ -9178,7 +9188,7 @@
         <x:v>15</x:v>
       </x:c>
       <x:c r="C27" s="51" t="s">
-        <x:v>212</x:v>
+        <x:v>214</x:v>
       </x:c>
       <x:c r="D27" s="181" t="n">
         <x:v>0.18</x:v>
@@ -9192,7 +9202,7 @@
       </x:c>
       <x:c r="I27" s="514" t="s"/>
       <x:c r="J27" s="517" t="s">
-        <x:v>213</x:v>
+        <x:v>215</x:v>
       </x:c>
       <x:c r="K27" s="569" t="s"/>
       <x:c r="L27" s="519" t="s"/>
@@ -9203,7 +9213,7 @@
     </x:row>
     <x:row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <x:c r="A28" s="513" t="s">
-        <x:v>214</x:v>
+        <x:v>216</x:v>
       </x:c>
       <x:c r="F28" s="355" t="s"/>
       <x:c r="G28" s="585" t="s">
@@ -9214,7 +9224,7 @@
       </x:c>
       <x:c r="I28" s="355" t="s"/>
       <x:c r="J28" s="127" t="s">
-        <x:v>215</x:v>
+        <x:v>217</x:v>
       </x:c>
       <x:c r="K28" s="145">
         <x:f>'Data Input'!C23</x:f>
@@ -9225,21 +9235,21 @@
     </x:row>
     <x:row r="29" spans="1:21" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A29" s="513" t="s">
-        <x:v>216</x:v>
+        <x:v>218</x:v>
       </x:c>
       <x:c r="C29" s="602" t="s"/>
       <x:c r="D29" s="602" t="s"/>
       <x:c r="E29" s="512" t="s"/>
       <x:c r="F29" s="572" t="s"/>
       <x:c r="G29" s="585" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="H29" s="594" t="e">
         <x:f>O6-SUM(O7:O11)-H27</x:f>
       </x:c>
       <x:c r="I29" s="355" t="s"/>
       <x:c r="J29" s="130" t="s">
-        <x:v>217</x:v>
+        <x:v>219</x:v>
       </x:c>
       <x:c r="K29" s="147">
         <x:f>IF(Tables!K11&gt;4000,10000,0)</x:f>
@@ -9248,35 +9258,35 @@
     </x:row>
     <x:row r="30" spans="1:21" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A30" s="513" t="s">
-        <x:v>218</x:v>
+        <x:v>220</x:v>
       </x:c>
       <x:c r="C30" s="514" t="s"/>
       <x:c r="D30" s="512" t="s"/>
       <x:c r="E30" s="512" t="s"/>
       <x:c r="F30" s="514" t="s"/>
       <x:c r="G30" s="515" t="s">
-        <x:v>38</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="H30" s="516" t="e">
         <x:f>H29/H27</x:f>
       </x:c>
       <x:c r="I30" s="355" t="s"/>
       <x:c r="J30" s="517" t="s">
-        <x:v>96</x:v>
+        <x:v>98</x:v>
       </x:c>
       <x:c r="K30" s="518" t="s"/>
       <x:c r="L30" s="519" t="s"/>
     </x:row>
     <x:row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <x:c r="A31" s="513" t="s">
-        <x:v>219</x:v>
+        <x:v>221</x:v>
       </x:c>
       <x:c r="C31" s="514" t="s"/>
       <x:c r="D31" s="362" t="s"/>
       <x:c r="F31" s="514" t="s"/>
       <x:c r="I31" s="355" t="s"/>
       <x:c r="J31" s="127" t="s">
-        <x:v>125</x:v>
+        <x:v>127</x:v>
       </x:c>
       <x:c r="K31" s="145">
         <x:f>(O13/100)*0.45/12*P1</x:f>
@@ -9285,14 +9295,14 @@
     </x:row>
     <x:row r="32" spans="1:21" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <x:c r="A32" s="597" t="s">
-        <x:v>220</x:v>
+        <x:v>222</x:v>
       </x:c>
       <x:c r="F32" s="514" t="s"/>
       <x:c r="G32" s="362" t="s"/>
       <x:c r="H32" s="355" t="s"/>
       <x:c r="I32" s="355" t="s"/>
       <x:c r="J32" s="127" t="s">
-        <x:v>221</x:v>
+        <x:v>223</x:v>
       </x:c>
       <x:c r="K32" s="145">
         <x:f>'Data Input'!C9/12*'Data Input'!C24</x:f>
@@ -9305,7 +9315,7 @@
       <x:c r="H33" s="355" t="s"/>
       <x:c r="I33" s="355" t="s"/>
       <x:c r="J33" s="130" t="s">
-        <x:v>222</x:v>
+        <x:v>224</x:v>
       </x:c>
       <x:c r="K33" s="147">
         <x:f>(('Data Input'!C8*50)*'Data Input'!C8+('Data Input'!C8*200)+('Data Input'!C8*50*'Data Input'!C8)+('Data Input'!C8*200)+('Data Input'!C8*50*'Data Input'!C8))</x:f>

</xml_diff>